<commit_message>
Otomatik güncelleme: 2025-04-26 03:21:07
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-04-23</t>
+          <t>2025-04-26</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-04-23</t>
+          <t>2025-04-26</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-04-23</t>
+          <t>2025-04-26</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1812,7 +1812,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-04-23</t>
+          <t>2025-04-26</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-04-23</t>
+          <t>2025-04-26</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-04-23</t>
+          <t>2025-04-26</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1866,7 +1866,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C175"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4151,6 +4151,19 @@
       </c>
       <c r="C175" t="n">
         <v>45.36</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="10" t="n">
+        <v>45773</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>45.37</v>
       </c>
     </row>
   </sheetData>
@@ -4164,7 +4177,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C175"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6449,6 +6462,19 @@
       </c>
       <c r="C175" t="n">
         <v>47.56</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="10" t="n">
+        <v>45773</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>47.59</v>
       </c>
     </row>
   </sheetData>
@@ -6462,7 +6488,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C175"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8747,6 +8773,19 @@
       </c>
       <c r="C175" t="n">
         <v>46.5</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="10" t="n">
+        <v>45773</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>46.52</v>
       </c>
     </row>
   </sheetData>
@@ -8760,7 +8799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C175"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11045,6 +11084,19 @@
       </c>
       <c r="C175" t="n">
         <v>46.79</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="10" t="n">
+        <v>45773</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>46.82</v>
       </c>
     </row>
   </sheetData>
@@ -11058,7 +11110,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C175"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13343,6 +13395,19 @@
       </c>
       <c r="C175" t="n">
         <v>47.51</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="10" t="n">
+        <v>45773</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>47.54</v>
       </c>
     </row>
   </sheetData>
@@ -13356,7 +13421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C175"/>
+  <dimension ref="A1:C176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15641,6 +15706,19 @@
       </c>
       <c r="C175" t="n">
         <v>47.16</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="10" t="n">
+        <v>45773</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>47.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-03 03:26:29
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-04-26</t>
+          <t>2025-05-03</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-04-26</t>
+          <t>2025-05-03</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-04-26</t>
+          <t>2025-05-03</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1337,7 +1337,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-04-26</t>
+          <t>2025-05-03</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-04-26</t>
+          <t>2025-05-03</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-04-26</t>
+          <t>2025-05-03</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1391,7 +1391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3689,6 +3689,19 @@
       </c>
       <c r="C176" t="n">
         <v>45.37</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="8" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>45.38</v>
       </c>
     </row>
   </sheetData>
@@ -3702,7 +3715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6000,6 +6013,19 @@
       </c>
       <c r="C176" t="n">
         <v>47.59</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="8" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>47.6</v>
       </c>
     </row>
   </sheetData>
@@ -6013,7 +6039,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8311,6 +8337,19 @@
       </c>
       <c r="C176" t="n">
         <v>46.52</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="8" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>46.53</v>
       </c>
     </row>
   </sheetData>
@@ -8324,7 +8363,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10622,6 +10661,19 @@
       </c>
       <c r="C176" t="n">
         <v>46.82</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="8" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>46.83</v>
       </c>
     </row>
   </sheetData>
@@ -10635,7 +10687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12933,6 +12985,19 @@
       </c>
       <c r="C176" t="n">
         <v>47.54</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="8" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>47.55</v>
       </c>
     </row>
   </sheetData>
@@ -12946,7 +13011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C176"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15244,6 +15309,19 @@
       </c>
       <c r="C176" t="n">
         <v>47.2</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="8" t="n">
+        <v>45780</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>47.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-06 03:30:53
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-03</t>
+          <t>2025-05-06</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-03</t>
+          <t>2025-05-06</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-03</t>
+          <t>2025-05-06</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1337,7 +1337,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-03</t>
+          <t>2025-05-06</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-03</t>
+          <t>2025-05-06</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-03</t>
+          <t>2025-05-06</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1391,7 +1391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3701,6 +3701,19 @@
         </is>
       </c>
       <c r="C177" t="n">
+        <v>45.38</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="8" t="n">
+        <v>45783</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
         <v>45.38</v>
       </c>
     </row>
@@ -3715,7 +3728,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6025,6 +6038,19 @@
         </is>
       </c>
       <c r="C177" t="n">
+        <v>47.6</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="8" t="n">
+        <v>45783</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
         <v>47.6</v>
       </c>
     </row>
@@ -6039,7 +6065,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8349,6 +8375,19 @@
         </is>
       </c>
       <c r="C177" t="n">
+        <v>46.53</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="8" t="n">
+        <v>45783</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
         <v>46.53</v>
       </c>
     </row>
@@ -8363,7 +8402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10673,6 +10712,19 @@
         </is>
       </c>
       <c r="C177" t="n">
+        <v>46.83</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="8" t="n">
+        <v>45783</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
         <v>46.83</v>
       </c>
     </row>
@@ -10687,7 +10739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12997,6 +13049,19 @@
         </is>
       </c>
       <c r="C177" t="n">
+        <v>47.55</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="8" t="n">
+        <v>45783</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
         <v>47.55</v>
       </c>
     </row>
@@ -13011,7 +13076,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15321,6 +15386,19 @@
         </is>
       </c>
       <c r="C177" t="n">
+        <v>47.21</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="8" t="n">
+        <v>45783</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
         <v>47.21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-07 03:32:40
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -765,7 +765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="16">
       <c r="A16" s="8" t="n">
-        <v>45673</v>
+        <v>45784</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1198,17 +1198,17 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>47.24</v>
+        <v>44.2</v>
       </c>
       <c r="D16" t="n">
-        <v>0.05587840858292359</v>
+        <v>-0.05089113162980452</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05587840858292359</v>
+        <v>-0.05089113162980452</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa İade Toplama</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1217,28 +1217,55 @@
     </row>
     <row r="17">
       <c r="A17" s="8" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>47.24</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8" t="n">
         <v>45756</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Motorin UltraForce</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
         <v>44.26</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D18" t="n">
         <v>-0.06308213378492811</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E18" t="n">
         <v>-0.06308213378492811</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
         </is>
       </c>
-      <c r="G17" t="n">
+      <c r="G18" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -1286,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-06</t>
+          <t>2025-05-07</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1303,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-06</t>
+          <t>2025-05-07</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1320,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-06</t>
+          <t>2025-05-07</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1337,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-06</t>
+          <t>2025-05-07</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1354,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-06</t>
+          <t>2025-05-07</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1371,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-06</t>
+          <t>2025-05-07</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1391,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3715,6 +3742,19 @@
       </c>
       <c r="C178" t="n">
         <v>45.38</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="8" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>44.2</v>
       </c>
     </row>
   </sheetData>
@@ -3728,7 +3768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6052,6 +6092,19 @@
       </c>
       <c r="C178" t="n">
         <v>47.6</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="8" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>46.42</v>
       </c>
     </row>
   </sheetData>
@@ -6065,7 +6118,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8389,6 +8442,19 @@
       </c>
       <c r="C178" t="n">
         <v>46.53</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="8" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>45.35</v>
       </c>
     </row>
   </sheetData>
@@ -8402,7 +8468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10726,6 +10792,19 @@
       </c>
       <c r="C178" t="n">
         <v>46.83</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="8" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>45.65</v>
       </c>
     </row>
   </sheetData>
@@ -10739,7 +10818,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13063,6 +13142,19 @@
       </c>
       <c r="C178" t="n">
         <v>47.55</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="8" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>46.37</v>
       </c>
     </row>
   </sheetData>
@@ -13076,7 +13168,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15400,6 +15492,19 @@
       </c>
       <c r="C178" t="n">
         <v>47.21</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="8" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>46.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-13 03:34:19
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-07</t>
+          <t>2025-05-13</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-07</t>
+          <t>2025-05-13</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-07</t>
+          <t>2025-05-13</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-07</t>
+          <t>2025-05-13</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-07</t>
+          <t>2025-05-13</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-07</t>
+          <t>2025-05-13</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3755,6 +3755,19 @@
       </c>
       <c r="C179" t="n">
         <v>44.2</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="8" t="n">
+        <v>45790</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>44.23</v>
       </c>
     </row>
   </sheetData>
@@ -3768,7 +3781,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6105,6 +6118,19 @@
       </c>
       <c r="C179" t="n">
         <v>46.42</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="8" t="n">
+        <v>45790</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>46.45</v>
       </c>
     </row>
   </sheetData>
@@ -6118,7 +6144,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8455,6 +8481,19 @@
       </c>
       <c r="C179" t="n">
         <v>45.35</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="8" t="n">
+        <v>45790</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>45.38</v>
       </c>
     </row>
   </sheetData>
@@ -8468,7 +8507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10805,6 +10844,19 @@
       </c>
       <c r="C179" t="n">
         <v>45.65</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="8" t="n">
+        <v>45790</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>45.68</v>
       </c>
     </row>
   </sheetData>
@@ -10818,7 +10870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13155,6 +13207,19 @@
       </c>
       <c r="C179" t="n">
         <v>46.37</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="8" t="n">
+        <v>45790</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>46.4</v>
       </c>
     </row>
   </sheetData>
@@ -13168,7 +13233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15505,6 +15570,19 @@
       </c>
       <c r="C179" t="n">
         <v>46.03</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="8" t="n">
+        <v>45790</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>46.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-14 03:33:06
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-13</t>
+          <t>2025-05-14</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-13</t>
+          <t>2025-05-14</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-13</t>
+          <t>2025-05-14</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-13</t>
+          <t>2025-05-14</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-13</t>
+          <t>2025-05-14</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-13</t>
+          <t>2025-05-14</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C180"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3767,6 +3767,19 @@
         </is>
       </c>
       <c r="C180" t="n">
+        <v>44.23</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="8" t="n">
+        <v>45791</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
         <v>44.23</v>
       </c>
     </row>
@@ -3781,7 +3794,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C180"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6130,6 +6143,19 @@
         </is>
       </c>
       <c r="C180" t="n">
+        <v>46.45</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="8" t="n">
+        <v>45791</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
         <v>46.45</v>
       </c>
     </row>
@@ -6144,7 +6170,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C180"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8493,6 +8519,19 @@
         </is>
       </c>
       <c r="C180" t="n">
+        <v>45.38</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="8" t="n">
+        <v>45791</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
         <v>45.38</v>
       </c>
     </row>
@@ -8507,7 +8546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C180"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10856,6 +10895,19 @@
         </is>
       </c>
       <c r="C180" t="n">
+        <v>45.68</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="8" t="n">
+        <v>45791</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
         <v>45.68</v>
       </c>
     </row>
@@ -10870,7 +10922,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C180"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13219,6 +13271,19 @@
         </is>
       </c>
       <c r="C180" t="n">
+        <v>46.4</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="8" t="n">
+        <v>45791</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
         <v>46.4</v>
       </c>
     </row>
@@ -13233,7 +13298,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C180"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15582,6 +15647,19 @@
         </is>
       </c>
       <c r="C180" t="n">
+        <v>46.06</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="8" t="n">
+        <v>45791</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
         <v>46.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-15 03:33:27
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-14</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-14</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-14</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-14</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-14</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-14</t>
+          <t>2025-05-15</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3781,6 +3781,19 @@
       </c>
       <c r="C181" t="n">
         <v>44.23</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="8" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>46.05</v>
       </c>
     </row>
   </sheetData>
@@ -3794,7 +3807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6157,6 +6170,19 @@
       </c>
       <c r="C181" t="n">
         <v>46.45</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="8" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>48.27</v>
       </c>
     </row>
   </sheetData>
@@ -6170,7 +6196,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8533,6 +8559,19 @@
       </c>
       <c r="C181" t="n">
         <v>45.38</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="8" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>47.2</v>
       </c>
     </row>
   </sheetData>
@@ -8546,7 +8585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10909,6 +10948,19 @@
       </c>
       <c r="C181" t="n">
         <v>45.68</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="8" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>47.5</v>
       </c>
     </row>
   </sheetData>
@@ -10922,7 +10974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13285,6 +13337,19 @@
       </c>
       <c r="C181" t="n">
         <v>46.4</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="8" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>48.22</v>
       </c>
     </row>
   </sheetData>
@@ -13298,7 +13363,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15661,6 +15726,19 @@
       </c>
       <c r="C181" t="n">
         <v>46.06</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="8" t="n">
+        <v>45792</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>47.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-16 03:34:57
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-15</t>
+          <t>2025-05-16</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-15</t>
+          <t>2025-05-16</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-15</t>
+          <t>2025-05-16</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-15</t>
+          <t>2025-05-16</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-15</t>
+          <t>2025-05-16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-15</t>
+          <t>2025-05-16</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3793,6 +3793,19 @@
         </is>
       </c>
       <c r="C182" t="n">
+        <v>46.05</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="8" t="n">
+        <v>45793</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
         <v>46.05</v>
       </c>
     </row>
@@ -3807,7 +3820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6182,6 +6195,19 @@
         </is>
       </c>
       <c r="C182" t="n">
+        <v>48.27</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="8" t="n">
+        <v>45793</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
         <v>48.27</v>
       </c>
     </row>
@@ -6196,7 +6222,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8571,6 +8597,19 @@
         </is>
       </c>
       <c r="C182" t="n">
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="8" t="n">
+        <v>45793</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
         <v>47.2</v>
       </c>
     </row>
@@ -8585,7 +8624,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10960,6 +10999,19 @@
         </is>
       </c>
       <c r="C182" t="n">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="8" t="n">
+        <v>45793</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
         <v>47.5</v>
       </c>
     </row>
@@ -10974,7 +11026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13349,6 +13401,19 @@
         </is>
       </c>
       <c r="C182" t="n">
+        <v>48.22</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="8" t="n">
+        <v>45793</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
         <v>48.22</v>
       </c>
     </row>
@@ -13363,7 +13428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15738,6 +15803,19 @@
         </is>
       </c>
       <c r="C182" t="n">
+        <v>47.88</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="8" t="n">
+        <v>45793</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
         <v>47.88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-17 03:29:53
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-16</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-16</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-16</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-16</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-16</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-16</t>
+          <t>2025-05-17</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3807,6 +3807,19 @@
       </c>
       <c r="C183" t="n">
         <v>46.05</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="8" t="n">
+        <v>45794</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>46.11</v>
       </c>
     </row>
   </sheetData>
@@ -3820,7 +3833,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6209,6 +6222,19 @@
       </c>
       <c r="C183" t="n">
         <v>48.27</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="8" t="n">
+        <v>45794</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>48.34</v>
       </c>
     </row>
   </sheetData>
@@ -6222,7 +6248,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8611,6 +8637,19 @@
       </c>
       <c r="C183" t="n">
         <v>47.2</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="8" t="n">
+        <v>45794</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>47.29</v>
       </c>
     </row>
   </sheetData>
@@ -8624,7 +8663,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11013,6 +11052,19 @@
       </c>
       <c r="C183" t="n">
         <v>47.5</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="8" t="n">
+        <v>45794</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>47.57</v>
       </c>
     </row>
   </sheetData>
@@ -11026,7 +11078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13415,6 +13467,19 @@
       </c>
       <c r="C183" t="n">
         <v>48.22</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="8" t="n">
+        <v>45794</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>48.29</v>
       </c>
     </row>
   </sheetData>
@@ -13428,7 +13493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15817,6 +15882,19 @@
       </c>
       <c r="C183" t="n">
         <v>47.88</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="8" t="n">
+        <v>45794</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>47.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-24 02:23:58
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-17</t>
+          <t>2025-05-24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-17</t>
+          <t>2025-05-24</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-17</t>
+          <t>2025-05-24</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-17</t>
+          <t>2025-05-24</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-17</t>
+          <t>2025-05-24</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-17</t>
+          <t>2025-05-24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3819,6 +3819,19 @@
         </is>
       </c>
       <c r="C184" t="n">
+        <v>46.11</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="8" t="n">
+        <v>45801</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
         <v>46.11</v>
       </c>
     </row>
@@ -3833,7 +3846,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6235,6 +6248,19 @@
       </c>
       <c r="C184" t="n">
         <v>48.34</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="8" t="n">
+        <v>45801</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>48.37</v>
       </c>
     </row>
   </sheetData>
@@ -6248,7 +6274,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8650,6 +8676,19 @@
       </c>
       <c r="C184" t="n">
         <v>47.29</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="8" t="n">
+        <v>45801</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>47.32</v>
       </c>
     </row>
   </sheetData>
@@ -8663,7 +8702,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11065,6 +11104,19 @@
       </c>
       <c r="C184" t="n">
         <v>47.57</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="8" t="n">
+        <v>45801</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>47.59</v>
       </c>
     </row>
   </sheetData>
@@ -11078,7 +11130,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13480,6 +13532,19 @@
       </c>
       <c r="C184" t="n">
         <v>48.29</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="8" t="n">
+        <v>45801</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>48.32</v>
       </c>
     </row>
   </sheetData>
@@ -13493,7 +13558,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15895,6 +15960,19 @@
       </c>
       <c r="C184" t="n">
         <v>47.96</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="8" t="n">
+        <v>45801</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>47.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-27 02:28:14
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-24</t>
+          <t>2025-05-27</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-24</t>
+          <t>2025-05-27</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-24</t>
+          <t>2025-05-27</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-24</t>
+          <t>2025-05-27</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-24</t>
+          <t>2025-05-27</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-24</t>
+          <t>2025-05-27</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3832,6 +3832,19 @@
         </is>
       </c>
       <c r="C185" t="n">
+        <v>46.11</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="8" t="n">
+        <v>45804</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
         <v>46.11</v>
       </c>
     </row>
@@ -3846,7 +3859,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6261,6 +6274,19 @@
       </c>
       <c r="C185" t="n">
         <v>48.37</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="8" t="n">
+        <v>45804</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>48.34</v>
       </c>
     </row>
   </sheetData>
@@ -6274,7 +6300,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8689,6 +8715,19 @@
       </c>
       <c r="C185" t="n">
         <v>47.32</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="8" t="n">
+        <v>45804</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>47.29</v>
       </c>
     </row>
   </sheetData>
@@ -8702,7 +8741,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11117,6 +11156,19 @@
       </c>
       <c r="C185" t="n">
         <v>47.59</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="8" t="n">
+        <v>45804</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>47.57</v>
       </c>
     </row>
   </sheetData>
@@ -11130,7 +11182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13545,6 +13597,19 @@
       </c>
       <c r="C185" t="n">
         <v>48.32</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="8" t="n">
+        <v>45804</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>48.29</v>
       </c>
     </row>
   </sheetData>
@@ -13558,7 +13623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C185"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15973,6 +16038,19 @@
       </c>
       <c r="C185" t="n">
         <v>47.99</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="8" t="n">
+        <v>45804</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>47.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-05-28 02:30:05
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3845,6 +3845,19 @@
         </is>
       </c>
       <c r="C186" t="n">
+        <v>46.11</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="8" t="n">
+        <v>45805</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
         <v>46.11</v>
       </c>
     </row>
@@ -3859,7 +3872,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6286,6 +6299,19 @@
         </is>
       </c>
       <c r="C186" t="n">
+        <v>48.34</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="8" t="n">
+        <v>45805</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
         <v>48.34</v>
       </c>
     </row>
@@ -6300,7 +6326,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8727,6 +8753,19 @@
         </is>
       </c>
       <c r="C186" t="n">
+        <v>47.29</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="8" t="n">
+        <v>45805</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
         <v>47.29</v>
       </c>
     </row>
@@ -8741,7 +8780,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11168,6 +11207,19 @@
         </is>
       </c>
       <c r="C186" t="n">
+        <v>47.57</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="8" t="n">
+        <v>45805</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
         <v>47.57</v>
       </c>
     </row>
@@ -11182,7 +11234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13609,6 +13661,19 @@
         </is>
       </c>
       <c r="C186" t="n">
+        <v>48.29</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="8" t="n">
+        <v>45805</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
         <v>48.29</v>
       </c>
     </row>
@@ -13623,7 +13688,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16050,6 +16115,19 @@
         </is>
       </c>
       <c r="C186" t="n">
+        <v>47.96</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="8" t="n">
+        <v>45805</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
         <v>47.96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-03 02:39:49
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-05-28</t>
+          <t>2025-06-03</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-05-28</t>
+          <t>2025-06-03</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-05-28</t>
+          <t>2025-06-03</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-05-28</t>
+          <t>2025-06-03</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-05-28</t>
+          <t>2025-06-03</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-05-28</t>
+          <t>2025-06-03</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3859,6 +3859,19 @@
       </c>
       <c r="C187" t="n">
         <v>46.11</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="8" t="n">
+        <v>45811</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>46.19</v>
       </c>
     </row>
   </sheetData>
@@ -3872,7 +3885,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6313,6 +6326,19 @@
       </c>
       <c r="C187" t="n">
         <v>48.34</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="8" t="n">
+        <v>45811</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>48.44</v>
       </c>
     </row>
   </sheetData>
@@ -6326,7 +6352,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8767,6 +8793,19 @@
       </c>
       <c r="C187" t="n">
         <v>47.29</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="8" t="n">
+        <v>45811</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>47.39</v>
       </c>
     </row>
   </sheetData>
@@ -8780,7 +8819,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11221,6 +11260,19 @@
       </c>
       <c r="C187" t="n">
         <v>47.57</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="8" t="n">
+        <v>45811</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>47.67</v>
       </c>
     </row>
   </sheetData>
@@ -11234,7 +11286,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13675,6 +13727,19 @@
       </c>
       <c r="C187" t="n">
         <v>48.29</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="8" t="n">
+        <v>45811</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>48.39</v>
       </c>
     </row>
   </sheetData>
@@ -13688,7 +13753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16129,6 +16194,19 @@
       </c>
       <c r="C187" t="n">
         <v>47.96</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="8" t="n">
+        <v>45811</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>48.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-06 02:38:54
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-03</t>
+          <t>2025-06-06</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-03</t>
+          <t>2025-06-06</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-03</t>
+          <t>2025-06-06</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-03</t>
+          <t>2025-06-06</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-03</t>
+          <t>2025-06-06</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-03</t>
+          <t>2025-06-06</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C188"/>
+  <dimension ref="A1:C189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3872,6 +3872,19 @@
       </c>
       <c r="C188" t="n">
         <v>46.19</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="8" t="n">
+        <v>45814</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>46.22</v>
       </c>
     </row>
   </sheetData>
@@ -3885,7 +3898,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C188"/>
+  <dimension ref="A1:C189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6339,6 +6352,19 @@
       </c>
       <c r="C188" t="n">
         <v>48.44</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="8" t="n">
+        <v>45814</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>48.47</v>
       </c>
     </row>
   </sheetData>
@@ -6352,7 +6378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C188"/>
+  <dimension ref="A1:C189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8806,6 +8832,19 @@
       </c>
       <c r="C188" t="n">
         <v>47.39</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="8" t="n">
+        <v>45814</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>47.42</v>
       </c>
     </row>
   </sheetData>
@@ -8819,7 +8858,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C188"/>
+  <dimension ref="A1:C189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11273,6 +11312,19 @@
       </c>
       <c r="C188" t="n">
         <v>47.67</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="8" t="n">
+        <v>45814</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>47.7</v>
       </c>
     </row>
   </sheetData>
@@ -11286,7 +11338,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C188"/>
+  <dimension ref="A1:C189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13740,6 +13792,19 @@
       </c>
       <c r="C188" t="n">
         <v>48.39</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="8" t="n">
+        <v>45814</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>48.42</v>
       </c>
     </row>
   </sheetData>
@@ -13753,7 +13818,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C188"/>
+  <dimension ref="A1:C189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16207,6 +16272,19 @@
       </c>
       <c r="C188" t="n">
         <v>48.06</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="8" t="n">
+        <v>45814</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>48.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-11 02:41:16
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-11</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-11</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-11</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-11</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-11</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-06</t>
+          <t>2025-06-11</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3884,6 +3884,19 @@
         </is>
       </c>
       <c r="C189" t="n">
+        <v>46.22</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="8" t="n">
+        <v>45819</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
         <v>46.22</v>
       </c>
     </row>
@@ -3898,7 +3911,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6364,6 +6377,19 @@
         </is>
       </c>
       <c r="C189" t="n">
+        <v>48.47</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="8" t="n">
+        <v>45819</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
         <v>48.47</v>
       </c>
     </row>
@@ -6378,7 +6404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8844,6 +8870,19 @@
         </is>
       </c>
       <c r="C189" t="n">
+        <v>47.42</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="8" t="n">
+        <v>45819</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
         <v>47.42</v>
       </c>
     </row>
@@ -8858,7 +8897,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11324,6 +11363,19 @@
         </is>
       </c>
       <c r="C189" t="n">
+        <v>47.7</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="8" t="n">
+        <v>45819</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
         <v>47.7</v>
       </c>
     </row>
@@ -11338,7 +11390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13804,6 +13856,19 @@
         </is>
       </c>
       <c r="C189" t="n">
+        <v>48.42</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="8" t="n">
+        <v>45819</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
         <v>48.42</v>
       </c>
     </row>
@@ -13818,7 +13883,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C189"/>
+  <dimension ref="A1:C190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16284,6 +16349,19 @@
         </is>
       </c>
       <c r="C189" t="n">
+        <v>48.1</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="8" t="n">
+        <v>45819</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
         <v>48.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-12 02:40:09
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-11</t>
+          <t>2025-06-12</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11</t>
+          <t>2025-06-12</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-11</t>
+          <t>2025-06-12</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-11</t>
+          <t>2025-06-12</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-11</t>
+          <t>2025-06-12</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-11</t>
+          <t>2025-06-12</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3898,6 +3898,19 @@
       </c>
       <c r="C190" t="n">
         <v>46.22</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="8" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>46.27</v>
       </c>
     </row>
   </sheetData>
@@ -3911,7 +3924,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6391,6 +6404,19 @@
       </c>
       <c r="C190" t="n">
         <v>48.47</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="8" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>48.52</v>
       </c>
     </row>
   </sheetData>
@@ -6404,7 +6430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8884,6 +8910,19 @@
       </c>
       <c r="C190" t="n">
         <v>47.42</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="8" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>47.47</v>
       </c>
     </row>
   </sheetData>
@@ -8897,7 +8936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11377,6 +11416,19 @@
       </c>
       <c r="C190" t="n">
         <v>47.7</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="8" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>47.75</v>
       </c>
     </row>
   </sheetData>
@@ -11390,7 +11442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13870,6 +13922,19 @@
       </c>
       <c r="C190" t="n">
         <v>48.42</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="8" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>48.47</v>
       </c>
     </row>
   </sheetData>
@@ -13883,7 +13948,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C190"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16363,6 +16428,19 @@
       </c>
       <c r="C190" t="n">
         <v>48.1</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="8" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>48.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-13 02:41:33
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-12</t>
+          <t>2025-06-13</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12</t>
+          <t>2025-06-13</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-12</t>
+          <t>2025-06-13</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12</t>
+          <t>2025-06-13</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-12</t>
+          <t>2025-06-13</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-12</t>
+          <t>2025-06-13</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3910,6 +3910,19 @@
         </is>
       </c>
       <c r="C191" t="n">
+        <v>46.27</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="8" t="n">
+        <v>45821</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
         <v>46.27</v>
       </c>
     </row>
@@ -3924,7 +3937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6416,6 +6429,19 @@
         </is>
       </c>
       <c r="C191" t="n">
+        <v>48.52</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="8" t="n">
+        <v>45821</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
         <v>48.52</v>
       </c>
     </row>
@@ -6430,7 +6456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8922,6 +8948,19 @@
         </is>
       </c>
       <c r="C191" t="n">
+        <v>47.47</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="8" t="n">
+        <v>45821</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
         <v>47.47</v>
       </c>
     </row>
@@ -8936,7 +8975,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11428,6 +11467,19 @@
         </is>
       </c>
       <c r="C191" t="n">
+        <v>47.75</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="8" t="n">
+        <v>45821</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
         <v>47.75</v>
       </c>
     </row>
@@ -11442,7 +11494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13934,6 +13986,19 @@
         </is>
       </c>
       <c r="C191" t="n">
+        <v>48.47</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="8" t="n">
+        <v>45821</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
         <v>48.47</v>
       </c>
     </row>
@@ -13948,7 +14013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16440,6 +16505,19 @@
         </is>
       </c>
       <c r="C191" t="n">
+        <v>48.15</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="8" t="n">
+        <v>45821</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
         <v>48.15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-14 02:28:32
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -765,7 +765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -866,7 +866,7 @@
     </row>
     <row r="4">
       <c r="A4" s="8" t="n">
-        <v>45673</v>
+        <v>45822</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -874,17 +874,17 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>48.88</v>
+        <v>49.96</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05663640293990491</v>
+        <v>0.07718844329452357</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05663640293990491</v>
+        <v>0.07718844329452357</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Servis Kayseri</t>
+          <t>Servis Diyarbakır</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -893,7 +893,7 @@
     </row>
     <row r="5">
       <c r="A5" s="8" t="n">
-        <v>45756</v>
+        <v>45673</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -901,13 +901,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>46.03</v>
+        <v>48.88</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -920,7 +920,7 @@
     </row>
     <row r="6">
       <c r="A6" s="8" t="n">
-        <v>45673</v>
+        <v>45756</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -928,17 +928,17 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>48.57</v>
+        <v>46.03</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05678851174934718</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="E6" t="n">
-        <v>0.05678851174934718</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -947,7 +947,7 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="n">
-        <v>45756</v>
+        <v>45822</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -955,17 +955,17 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>45.66</v>
+        <v>49.64</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.05991352686843743</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.05991352686843743</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -982,17 +982,17 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>47.24</v>
+        <v>48.57</v>
       </c>
       <c r="D8" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="E8" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1009,17 +1009,17 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>44.26</v>
+        <v>45.66</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.06308213378492811</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.06308213378492811</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1028,7 +1028,7 @@
     </row>
     <row r="10">
       <c r="A10" s="8" t="n">
-        <v>45673</v>
+        <v>45822</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1036,17 +1036,17 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>47.24</v>
+        <v>49.24</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="E10" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -1055,7 +1055,7 @@
     </row>
     <row r="11">
       <c r="A11" s="8" t="n">
-        <v>45756</v>
+        <v>45673</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1063,17 +1063,17 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>44.26</v>
+        <v>47.24</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -1082,7 +1082,7 @@
     </row>
     <row r="12">
       <c r="A12" s="8" t="n">
-        <v>45673</v>
+        <v>45756</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1090,17 +1090,17 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>47.24</v>
+        <v>44.26</v>
       </c>
       <c r="D12" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E12" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -1109,7 +1109,7 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="n">
-        <v>45756</v>
+        <v>45822</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1117,17 +1117,17 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>44.26</v>
+        <v>47.76</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1190,7 +1190,7 @@
     </row>
     <row r="16">
       <c r="A16" s="8" t="n">
-        <v>45784</v>
+        <v>45822</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1198,17 +1198,17 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>44.2</v>
+        <v>47.76</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.05089113162980452</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.05089113162980452</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1228,14 +1228,14 @@
         <v>47.24</v>
       </c>
       <c r="D17" t="n">
-        <v>0.05587840858292359</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E17" t="n">
-        <v>0.05587840858292359</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1262,10 +1262,253 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>Spot Araç Teknosa</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Spot Araç Teknosa</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>47.24</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.07023108291798819</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.07023108291798819</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa Toplama</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="n">
+        <v>45756</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>44.26</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa Toplama</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa Toplama</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>44.2</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-0.05089113162980452</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0.05089113162980452</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0805429864253393</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0805429864253393</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>47.24</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
           <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="G25" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="n">
+        <v>45756</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>44.26</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -1313,7 +1556,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-13</t>
+          <t>2025-06-14</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1330,7 +1573,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13</t>
+          <t>2025-06-14</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1347,7 +1590,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-13</t>
+          <t>2025-06-14</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1364,7 +1607,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-13</t>
+          <t>2025-06-14</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1381,7 +1624,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-13</t>
+          <t>2025-06-14</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1398,7 +1641,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-13</t>
+          <t>2025-06-14</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1418,7 +1661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C192"/>
+  <dimension ref="A1:C193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3924,6 +4167,19 @@
       </c>
       <c r="C192" t="n">
         <v>46.27</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>47.76</v>
       </c>
     </row>
   </sheetData>
@@ -3937,7 +4193,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C192"/>
+  <dimension ref="A1:C193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6443,6 +6699,19 @@
       </c>
       <c r="C192" t="n">
         <v>48.52</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>50.01</v>
       </c>
     </row>
   </sheetData>
@@ -6456,7 +6725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C192"/>
+  <dimension ref="A1:C193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8962,6 +9231,19 @@
       </c>
       <c r="C192" t="n">
         <v>47.47</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>48.96</v>
       </c>
     </row>
   </sheetData>
@@ -8975,7 +9257,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C192"/>
+  <dimension ref="A1:C193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11481,6 +11763,19 @@
       </c>
       <c r="C192" t="n">
         <v>47.75</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>49.24</v>
       </c>
     </row>
   </sheetData>
@@ -11494,7 +11789,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C192"/>
+  <dimension ref="A1:C193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14000,6 +14295,19 @@
       </c>
       <c r="C192" t="n">
         <v>48.47</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>49.96</v>
       </c>
     </row>
   </sheetData>
@@ -14013,7 +14321,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C192"/>
+  <dimension ref="A1:C193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16519,6 +16827,19 @@
       </c>
       <c r="C192" t="n">
         <v>48.15</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>49.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-17 02:41:58
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-14</t>
+          <t>2025-06-17</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-14</t>
+          <t>2025-06-17</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-14</t>
+          <t>2025-06-17</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-14</t>
+          <t>2025-06-17</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-14</t>
+          <t>2025-06-17</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-14</t>
+          <t>2025-06-17</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1661,7 +1661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4180,6 +4180,19 @@
       </c>
       <c r="C193" t="n">
         <v>47.76</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="8" t="n">
+        <v>45825</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>49.5</v>
       </c>
     </row>
   </sheetData>
@@ -4193,7 +4206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6712,6 +6725,19 @@
       </c>
       <c r="C193" t="n">
         <v>50.01</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="8" t="n">
+        <v>45825</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>51.75</v>
       </c>
     </row>
   </sheetData>
@@ -6725,7 +6751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9244,6 +9270,19 @@
       </c>
       <c r="C193" t="n">
         <v>48.96</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="8" t="n">
+        <v>45825</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>50.7</v>
       </c>
     </row>
   </sheetData>
@@ -9257,7 +9296,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11776,6 +11815,19 @@
       </c>
       <c r="C193" t="n">
         <v>49.24</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="8" t="n">
+        <v>45825</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>50.98</v>
       </c>
     </row>
   </sheetData>
@@ -11789,7 +11841,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14308,6 +14360,19 @@
       </c>
       <c r="C193" t="n">
         <v>49.96</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="8" t="n">
+        <v>45825</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>51.7</v>
       </c>
     </row>
   </sheetData>
@@ -14321,7 +14386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C193"/>
+  <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16840,6 +16905,19 @@
       </c>
       <c r="C193" t="n">
         <v>49.64</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="8" t="n">
+        <v>45825</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>51.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-19 02:42:11
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -765,7 +765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,7 +893,7 @@
     </row>
     <row r="5">
       <c r="A5" s="8" t="n">
-        <v>45673</v>
+        <v>45827</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -901,17 +901,17 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>48.88</v>
+        <v>53.57</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05663640293990491</v>
+        <v>0.07225780624499589</v>
       </c>
       <c r="E5" t="n">
-        <v>0.05663640293990491</v>
+        <v>0.07225780624499589</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Servis Kayseri</t>
+          <t>Servis Diyarbakır</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -920,7 +920,7 @@
     </row>
     <row r="6">
       <c r="A6" s="8" t="n">
-        <v>45756</v>
+        <v>45673</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -928,13 +928,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>46.03</v>
+        <v>48.88</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -947,7 +947,7 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="n">
-        <v>45822</v>
+        <v>45756</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -955,13 +955,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>49.64</v>
+        <v>46.03</v>
       </c>
       <c r="D7" t="n">
-        <v>0.07842711275255265</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="E7" t="n">
-        <v>0.07842711275255265</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -974,7 +974,7 @@
     </row>
     <row r="8">
       <c r="A8" s="8" t="n">
-        <v>45673</v>
+        <v>45822</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -982,17 +982,17 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>48.57</v>
+        <v>49.64</v>
       </c>
       <c r="D8" t="n">
-        <v>0.05678851174934718</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="E8" t="n">
-        <v>0.05678851174934718</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1001,7 +1001,7 @@
     </row>
     <row r="9">
       <c r="A9" s="8" t="n">
-        <v>45756</v>
+        <v>45827</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1009,17 +1009,17 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>45.66</v>
+        <v>53.25</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.05991352686843743</v>
+        <v>0.07272360999194194</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.05991352686843743</v>
+        <v>0.07272360999194194</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1028,7 +1028,7 @@
     </row>
     <row r="10">
       <c r="A10" s="8" t="n">
-        <v>45822</v>
+        <v>45673</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>49.24</v>
+        <v>48.57</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07840560665790641</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="E10" t="n">
-        <v>0.07840560665790641</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="11">
       <c r="A11" s="8" t="n">
-        <v>45673</v>
+        <v>45756</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1063,17 +1063,17 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>47.24</v>
+        <v>45.66</v>
       </c>
       <c r="D11" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="E11" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -1082,7 +1082,7 @@
     </row>
     <row r="12">
       <c r="A12" s="8" t="n">
-        <v>45756</v>
+        <v>45822</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1090,17 +1090,17 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>44.26</v>
+        <v>49.24</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -1109,7 +1109,7 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="n">
-        <v>45822</v>
+        <v>45827</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1117,17 +1117,17 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>47.76</v>
+        <v>52.85</v>
       </c>
       <c r="D13" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07331437855402112</v>
       </c>
       <c r="E13" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07331437855402112</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1217,7 +1217,7 @@
     </row>
     <row r="17">
       <c r="A17" s="8" t="n">
-        <v>45673</v>
+        <v>45827</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1225,17 +1225,17 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>47.24</v>
+        <v>51.37</v>
       </c>
       <c r="D17" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E17" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1244,7 +1244,7 @@
     </row>
     <row r="18">
       <c r="A18" s="8" t="n">
-        <v>45756</v>
+        <v>45673</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1252,17 +1252,17 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>44.26</v>
+        <v>47.24</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1271,7 +1271,7 @@
     </row>
     <row r="19">
       <c r="A19" s="8" t="n">
-        <v>45822</v>
+        <v>45756</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1279,17 +1279,17 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>47.76</v>
+        <v>44.26</v>
       </c>
       <c r="D19" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E19" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1298,7 +1298,7 @@
     </row>
     <row r="20">
       <c r="A20" s="8" t="n">
-        <v>45673</v>
+        <v>45822</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1306,17 +1306,17 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>47.24</v>
+        <v>47.76</v>
       </c>
       <c r="D20" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E20" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1325,7 +1325,7 @@
     </row>
     <row r="21">
       <c r="A21" s="8" t="n">
-        <v>45756</v>
+        <v>45827</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1333,17 +1333,17 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>44.26</v>
+        <v>51.37</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1352,7 +1352,7 @@
     </row>
     <row r="22">
       <c r="A22" s="8" t="n">
-        <v>45822</v>
+        <v>45673</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1360,17 +1360,17 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>47.76</v>
+        <v>47.24</v>
       </c>
       <c r="D22" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E22" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1379,7 +1379,7 @@
     </row>
     <row r="23">
       <c r="A23" s="8" t="n">
-        <v>45784</v>
+        <v>45756</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1387,17 +1387,17 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>44.2</v>
+        <v>44.26</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.05089113162980452</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.05089113162980452</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1417,14 +1417,14 @@
         <v>47.76</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0805429864253393</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0805429864253393</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1433,7 +1433,7 @@
     </row>
     <row r="25">
       <c r="A25" s="8" t="n">
-        <v>45673</v>
+        <v>45827</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1441,17 +1441,17 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>47.24</v>
+        <v>51.37</v>
       </c>
       <c r="D25" t="n">
-        <v>0.05587840858292359</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E25" t="n">
-        <v>0.05587840858292359</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1460,7 +1460,7 @@
     </row>
     <row r="26">
       <c r="A26" s="8" t="n">
-        <v>45756</v>
+        <v>45673</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1468,17 +1468,17 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>44.26</v>
+        <v>47.24</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1487,28 +1487,271 @@
     </row>
     <row r="27">
       <c r="A27" s="8" t="n">
+        <v>45756</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>44.26</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa Toplama</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="n">
         <v>45822</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Motorin UltraForce</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
         <v>47.76</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D28" t="n">
         <v>0.07907817442385912</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E28" t="n">
         <v>0.07907817442385912</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa Toplama</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>51.37</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa Toplama</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>44.2</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-0.05089113162980452</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-0.05089113162980452</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0805429864253393</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0805429864253393</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>51.37</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="8" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>47.24</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="F33" t="inlineStr">
         <is>
           <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
         </is>
       </c>
-      <c r="G27" t="n">
+      <c r="G33" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="n">
+        <v>45756</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>44.26</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>51.37</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -1556,7 +1799,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-17</t>
+          <t>2025-06-19</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1573,7 +1816,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-17</t>
+          <t>2025-06-19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1590,7 +1833,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-17</t>
+          <t>2025-06-19</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1607,7 +1850,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-17</t>
+          <t>2025-06-19</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1624,7 +1867,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-17</t>
+          <t>2025-06-19</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1641,7 +1884,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-17</t>
+          <t>2025-06-19</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1661,7 +1904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C194"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4193,6 +4436,19 @@
       </c>
       <c r="C194" t="n">
         <v>49.5</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>51.37</v>
       </c>
     </row>
   </sheetData>
@@ -4206,7 +4462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C194"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6738,6 +6994,19 @@
       </c>
       <c r="C194" t="n">
         <v>51.75</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>53.62</v>
       </c>
     </row>
   </sheetData>
@@ -6751,7 +7020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C194"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9283,6 +9552,19 @@
       </c>
       <c r="C194" t="n">
         <v>50.7</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>52.57</v>
       </c>
     </row>
   </sheetData>
@@ -9296,7 +9578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C194"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11828,6 +12110,19 @@
       </c>
       <c r="C194" t="n">
         <v>50.98</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>52.85</v>
       </c>
     </row>
   </sheetData>
@@ -11841,7 +12136,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C194"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14373,6 +14668,19 @@
       </c>
       <c r="C194" t="n">
         <v>51.7</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>53.57</v>
       </c>
     </row>
   </sheetData>
@@ -14386,7 +14694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C194"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16918,6 +17226,19 @@
       </c>
       <c r="C194" t="n">
         <v>51.38</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>53.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-21 02:29:20
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -765,7 +765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -920,7 +920,7 @@
     </row>
     <row r="6">
       <c r="A6" s="8" t="n">
-        <v>45673</v>
+        <v>45829</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -928,17 +928,17 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>48.88</v>
+        <v>56.91</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05663640293990491</v>
+        <v>0.06234832928878098</v>
       </c>
       <c r="E6" t="n">
-        <v>0.05663640293990491</v>
+        <v>0.06234832928878098</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Servis Kayseri</t>
+          <t>Servis Diyarbakır</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -947,7 +947,7 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="n">
-        <v>45756</v>
+        <v>45673</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -955,13 +955,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>46.03</v>
+        <v>48.88</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -974,7 +974,7 @@
     </row>
     <row r="8">
       <c r="A8" s="8" t="n">
-        <v>45822</v>
+        <v>45756</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -982,13 +982,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>49.64</v>
+        <v>46.03</v>
       </c>
       <c r="D8" t="n">
-        <v>0.07842711275255265</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="E8" t="n">
-        <v>0.07842711275255265</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1001,7 +1001,7 @@
     </row>
     <row r="9">
       <c r="A9" s="8" t="n">
-        <v>45827</v>
+        <v>45822</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1009,13 +1009,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>53.25</v>
+        <v>49.64</v>
       </c>
       <c r="D9" t="n">
-        <v>0.07272360999194194</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="E9" t="n">
-        <v>0.07272360999194194</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="10">
       <c r="A10" s="8" t="n">
-        <v>45673</v>
+        <v>45827</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1036,17 +1036,17 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>48.57</v>
+        <v>53.25</v>
       </c>
       <c r="D10" t="n">
-        <v>0.05678851174934718</v>
+        <v>0.07272360999194194</v>
       </c>
       <c r="E10" t="n">
-        <v>0.05678851174934718</v>
+        <v>0.07272360999194194</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -1055,7 +1055,7 @@
     </row>
     <row r="11">
       <c r="A11" s="8" t="n">
-        <v>45756</v>
+        <v>45829</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1063,17 +1063,17 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>45.66</v>
+        <v>56.59</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.05991352686843743</v>
+        <v>0.06272300469483572</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.05991352686843743</v>
+        <v>0.06272300469483572</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -1082,7 +1082,7 @@
     </row>
     <row r="12">
       <c r="A12" s="8" t="n">
-        <v>45822</v>
+        <v>45673</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1090,13 +1090,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>49.24</v>
+        <v>48.57</v>
       </c>
       <c r="D12" t="n">
-        <v>0.07840560665790641</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="E12" t="n">
-        <v>0.07840560665790641</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="n">
-        <v>45827</v>
+        <v>45756</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1117,13 +1117,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>52.85</v>
+        <v>45.66</v>
       </c>
       <c r="D13" t="n">
-        <v>0.07331437855402112</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="E13" t="n">
-        <v>0.07331437855402112</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="14">
       <c r="A14" s="8" t="n">
-        <v>45673</v>
+        <v>45822</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1144,17 +1144,17 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>47.24</v>
+        <v>49.24</v>
       </c>
       <c r="D14" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="E14" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -1163,7 +1163,7 @@
     </row>
     <row r="15">
       <c r="A15" s="8" t="n">
-        <v>45756</v>
+        <v>45827</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1171,17 +1171,17 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>44.26</v>
+        <v>52.85</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07331437855402112</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07331437855402112</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1190,7 +1190,7 @@
     </row>
     <row r="16">
       <c r="A16" s="8" t="n">
-        <v>45822</v>
+        <v>45829</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1198,17 +1198,17 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>47.76</v>
+        <v>56.19</v>
       </c>
       <c r="D16" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.06319772942289492</v>
       </c>
       <c r="E16" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.06319772942289492</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1217,7 +1217,7 @@
     </row>
     <row r="17">
       <c r="A17" s="8" t="n">
-        <v>45827</v>
+        <v>45673</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1225,13 +1225,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>51.37</v>
+        <v>47.24</v>
       </c>
       <c r="D17" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E17" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="18">
       <c r="A18" s="8" t="n">
-        <v>45673</v>
+        <v>45756</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1252,17 +1252,17 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>47.24</v>
+        <v>44.26</v>
       </c>
       <c r="D18" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E18" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1271,7 +1271,7 @@
     </row>
     <row r="19">
       <c r="A19" s="8" t="n">
-        <v>45756</v>
+        <v>45822</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1279,17 +1279,17 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>44.26</v>
+        <v>47.76</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1298,7 +1298,7 @@
     </row>
     <row r="20">
       <c r="A20" s="8" t="n">
-        <v>45822</v>
+        <v>45827</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1306,17 +1306,17 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>47.76</v>
+        <v>51.37</v>
       </c>
       <c r="D20" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E20" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1325,7 +1325,7 @@
     </row>
     <row r="21">
       <c r="A21" s="8" t="n">
-        <v>45827</v>
+        <v>45829</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1333,17 +1333,17 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>51.37</v>
+        <v>54.71</v>
       </c>
       <c r="D21" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E21" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1424,7 +1424,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1460,7 +1460,7 @@
     </row>
     <row r="26">
       <c r="A26" s="8" t="n">
-        <v>45673</v>
+        <v>45829</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1468,17 +1468,17 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>47.24</v>
+        <v>54.71</v>
       </c>
       <c r="D26" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E26" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1487,7 +1487,7 @@
     </row>
     <row r="27">
       <c r="A27" s="8" t="n">
-        <v>45756</v>
+        <v>45673</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1495,17 +1495,17 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>44.26</v>
+        <v>47.24</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1514,7 +1514,7 @@
     </row>
     <row r="28">
       <c r="A28" s="8" t="n">
-        <v>45822</v>
+        <v>45756</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1522,17 +1522,17 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>47.76</v>
+        <v>44.26</v>
       </c>
       <c r="D28" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E28" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1541,7 +1541,7 @@
     </row>
     <row r="29">
       <c r="A29" s="8" t="n">
-        <v>45827</v>
+        <v>45822</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1549,17 +1549,17 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>51.37</v>
+        <v>47.76</v>
       </c>
       <c r="D29" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E29" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1568,7 +1568,7 @@
     </row>
     <row r="30">
       <c r="A30" s="8" t="n">
-        <v>45784</v>
+        <v>45827</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1576,17 +1576,17 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>44.2</v>
+        <v>51.37</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.05089113162980452</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.05089113162980452</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1595,7 +1595,7 @@
     </row>
     <row r="31">
       <c r="A31" s="8" t="n">
-        <v>45822</v>
+        <v>45829</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1603,17 +1603,17 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>47.76</v>
+        <v>54.71</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0805429864253393</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0805429864253393</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1622,7 +1622,7 @@
     </row>
     <row r="32">
       <c r="A32" s="8" t="n">
-        <v>45827</v>
+        <v>45673</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1630,17 +1630,17 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>51.37</v>
+        <v>47.24</v>
       </c>
       <c r="D32" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E32" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -1649,7 +1649,7 @@
     </row>
     <row r="33">
       <c r="A33" s="8" t="n">
-        <v>45673</v>
+        <v>45756</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1657,17 +1657,17 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>47.24</v>
+        <v>44.26</v>
       </c>
       <c r="D33" t="n">
-        <v>0.05587840858292359</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E33" t="n">
-        <v>0.05587840858292359</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -1676,7 +1676,7 @@
     </row>
     <row r="34">
       <c r="A34" s="8" t="n">
-        <v>45756</v>
+        <v>45822</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1684,17 +1684,17 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>44.26</v>
+        <v>47.76</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1703,7 +1703,7 @@
     </row>
     <row r="35">
       <c r="A35" s="8" t="n">
-        <v>45822</v>
+        <v>45827</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1711,17 +1711,17 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>47.76</v>
+        <v>51.37</v>
       </c>
       <c r="D35" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E35" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1730,28 +1730,271 @@
     </row>
     <row r="36">
       <c r="A36" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>54.71</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa Toplama</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="n">
+        <v>45784</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>44.2</v>
+      </c>
+      <c r="D37" t="n">
+        <v>-0.05089113162980452</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-0.05089113162980452</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0805429864253393</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.0805429864253393</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="8" t="n">
         <v>45827</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Motorin UltraForce</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
         <v>51.37</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D39" t="n">
         <v>0.07558626465661633</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E39" t="n">
         <v>0.07558626465661633</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>54.71</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="8" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>47.24</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="F41" t="inlineStr">
         <is>
           <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
         </is>
       </c>
-      <c r="G36" t="n">
+      <c r="G41" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="8" t="n">
+        <v>45756</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>44.26</v>
+      </c>
+      <c r="D42" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>51.37</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>54.71</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -1799,7 +2042,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-06-21</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1816,7 +2059,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-06-21</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1833,7 +2076,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-06-21</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1850,7 +2093,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-06-21</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1867,7 +2110,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-06-21</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1884,7 +2127,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-06-21</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1904,7 +2147,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4449,6 +4692,19 @@
       </c>
       <c r="C195" t="n">
         <v>51.37</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>54.71</v>
       </c>
     </row>
   </sheetData>
@@ -4462,7 +4718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7007,6 +7263,19 @@
       </c>
       <c r="C195" t="n">
         <v>53.62</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>56.96</v>
       </c>
     </row>
   </sheetData>
@@ -7020,7 +7289,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9565,6 +9834,19 @@
       </c>
       <c r="C195" t="n">
         <v>52.57</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>55.91</v>
       </c>
     </row>
   </sheetData>
@@ -9578,7 +9860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12123,6 +12405,19 @@
       </c>
       <c r="C195" t="n">
         <v>52.85</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>56.19</v>
       </c>
     </row>
   </sheetData>
@@ -12136,7 +12431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14681,6 +14976,19 @@
       </c>
       <c r="C195" t="n">
         <v>53.57</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>56.91</v>
       </c>
     </row>
   </sheetData>
@@ -14694,7 +15002,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17239,6 +17547,19 @@
       </c>
       <c r="C195" t="n">
         <v>53.25</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>56.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-24 02:42:43
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2042,7 +2042,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-21</t>
+          <t>2025-06-24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2059,7 +2059,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-21</t>
+          <t>2025-06-24</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-21</t>
+          <t>2025-06-24</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-21</t>
+          <t>2025-06-24</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-21</t>
+          <t>2025-06-24</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2127,7 +2127,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-21</t>
+          <t>2025-06-24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2147,7 +2147,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4705,6 +4705,19 @@
       </c>
       <c r="C196" t="n">
         <v>54.71</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="8" t="n">
+        <v>45832</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>53.05</v>
       </c>
     </row>
   </sheetData>
@@ -4718,7 +4731,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7276,6 +7289,19 @@
       </c>
       <c r="C196" t="n">
         <v>56.96</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="8" t="n">
+        <v>45832</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>55.3</v>
       </c>
     </row>
   </sheetData>
@@ -7289,7 +7315,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9847,6 +9873,19 @@
       </c>
       <c r="C196" t="n">
         <v>55.91</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="8" t="n">
+        <v>45832</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>54.25</v>
       </c>
     </row>
   </sheetData>
@@ -9860,7 +9899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12418,6 +12457,19 @@
       </c>
       <c r="C196" t="n">
         <v>56.19</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="8" t="n">
+        <v>45832</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>54.53</v>
       </c>
     </row>
   </sheetData>
@@ -12431,7 +12483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14989,6 +15041,19 @@
       </c>
       <c r="C196" t="n">
         <v>56.91</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="8" t="n">
+        <v>45832</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>55.25</v>
       </c>
     </row>
   </sheetData>
@@ -15002,7 +15067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17560,6 +17625,19 @@
       </c>
       <c r="C196" t="n">
         <v>56.59</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="8" t="n">
+        <v>45832</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>54.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-26 02:42:29
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -765,7 +765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -947,7 +947,7 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="n">
-        <v>45673</v>
+        <v>45834</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -955,17 +955,17 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>48.88</v>
+        <v>51.26</v>
       </c>
       <c r="D7" t="n">
-        <v>0.05663640293990491</v>
+        <v>-0.09927956422421369</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05663640293990491</v>
+        <v>-0.09927956422421369</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Servis Kayseri</t>
+          <t>Servis Diyarbakır</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -974,7 +974,7 @@
     </row>
     <row r="8">
       <c r="A8" s="8" t="n">
-        <v>45756</v>
+        <v>45673</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -982,13 +982,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>46.03</v>
+        <v>48.88</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1001,7 +1001,7 @@
     </row>
     <row r="9">
       <c r="A9" s="8" t="n">
-        <v>45822</v>
+        <v>45756</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1009,13 +1009,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>49.64</v>
+        <v>46.03</v>
       </c>
       <c r="D9" t="n">
-        <v>0.07842711275255265</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="E9" t="n">
-        <v>0.07842711275255265</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="10">
       <c r="A10" s="8" t="n">
-        <v>45827</v>
+        <v>45822</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>53.25</v>
+        <v>49.64</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07272360999194194</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="E10" t="n">
-        <v>0.07272360999194194</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="11">
       <c r="A11" s="8" t="n">
-        <v>45829</v>
+        <v>45827</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1063,13 +1063,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>56.59</v>
+        <v>53.25</v>
       </c>
       <c r="D11" t="n">
-        <v>0.06272300469483572</v>
+        <v>0.07272360999194194</v>
       </c>
       <c r="E11" t="n">
-        <v>0.06272300469483572</v>
+        <v>0.07272360999194194</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="12">
       <c r="A12" s="8" t="n">
-        <v>45673</v>
+        <v>45829</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1090,17 +1090,17 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>48.57</v>
+        <v>56.59</v>
       </c>
       <c r="D12" t="n">
-        <v>0.05678851174934718</v>
+        <v>0.06272300469483572</v>
       </c>
       <c r="E12" t="n">
-        <v>0.05678851174934718</v>
+        <v>0.06272300469483572</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -1109,7 +1109,7 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="n">
-        <v>45756</v>
+        <v>45834</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1117,17 +1117,17 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>45.66</v>
+        <v>50.94</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.05991352686843743</v>
+        <v>-0.09984096130058329</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.05991352686843743</v>
+        <v>-0.09984096130058329</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -1136,7 +1136,7 @@
     </row>
     <row r="14">
       <c r="A14" s="8" t="n">
-        <v>45822</v>
+        <v>45673</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1144,13 +1144,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>49.24</v>
+        <v>48.57</v>
       </c>
       <c r="D14" t="n">
-        <v>0.07840560665790641</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="E14" t="n">
-        <v>0.07840560665790641</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="15">
       <c r="A15" s="8" t="n">
-        <v>45827</v>
+        <v>45756</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1171,13 +1171,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>52.85</v>
+        <v>45.66</v>
       </c>
       <c r="D15" t="n">
-        <v>0.07331437855402112</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="E15" t="n">
-        <v>0.07331437855402112</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="16">
       <c r="A16" s="8" t="n">
-        <v>45829</v>
+        <v>45822</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1198,13 +1198,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>56.19</v>
+        <v>49.24</v>
       </c>
       <c r="D16" t="n">
-        <v>0.06319772942289492</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="E16" t="n">
-        <v>0.06319772942289492</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="17">
       <c r="A17" s="8" t="n">
-        <v>45673</v>
+        <v>45827</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1225,17 +1225,17 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>47.24</v>
+        <v>52.85</v>
       </c>
       <c r="D17" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07331437855402112</v>
       </c>
       <c r="E17" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07331437855402112</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1244,7 +1244,7 @@
     </row>
     <row r="18">
       <c r="A18" s="8" t="n">
-        <v>45756</v>
+        <v>45829</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1252,17 +1252,17 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>44.26</v>
+        <v>56.19</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.06319772942289492</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.06319772942289492</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1271,7 +1271,7 @@
     </row>
     <row r="19">
       <c r="A19" s="8" t="n">
-        <v>45822</v>
+        <v>45834</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1279,17 +1279,17 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>47.76</v>
+        <v>50.54</v>
       </c>
       <c r="D19" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.1005516995906744</v>
       </c>
       <c r="E19" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.1005516995906744</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1298,7 +1298,7 @@
     </row>
     <row r="20">
       <c r="A20" s="8" t="n">
-        <v>45827</v>
+        <v>45673</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1306,13 +1306,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>51.37</v>
+        <v>47.24</v>
       </c>
       <c r="D20" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E20" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="21">
       <c r="A21" s="8" t="n">
-        <v>45829</v>
+        <v>45756</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1333,13 +1333,13 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>54.71</v>
+        <v>44.26</v>
       </c>
       <c r="D21" t="n">
-        <v>0.06501849328401788</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E21" t="n">
-        <v>0.06501849328401788</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="22">
       <c r="A22" s="8" t="n">
-        <v>45673</v>
+        <v>45822</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1360,17 +1360,17 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>47.24</v>
+        <v>47.76</v>
       </c>
       <c r="D22" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E22" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1379,7 +1379,7 @@
     </row>
     <row r="23">
       <c r="A23" s="8" t="n">
-        <v>45756</v>
+        <v>45827</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1387,17 +1387,17 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>44.26</v>
+        <v>51.37</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1406,7 +1406,7 @@
     </row>
     <row r="24">
       <c r="A24" s="8" t="n">
-        <v>45822</v>
+        <v>45829</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1414,17 +1414,17 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>47.76</v>
+        <v>54.71</v>
       </c>
       <c r="D24" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E24" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1433,7 +1433,7 @@
     </row>
     <row r="25">
       <c r="A25" s="8" t="n">
-        <v>45827</v>
+        <v>45834</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1441,17 +1441,17 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>51.37</v>
+        <v>49.06</v>
       </c>
       <c r="D25" t="n">
-        <v>0.07558626465661633</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="E25" t="n">
-        <v>0.07558626465661633</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1460,7 +1460,7 @@
     </row>
     <row r="26">
       <c r="A26" s="8" t="n">
-        <v>45829</v>
+        <v>45673</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1468,13 +1468,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>54.71</v>
+        <v>47.24</v>
       </c>
       <c r="D26" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E26" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="27">
       <c r="A27" s="8" t="n">
-        <v>45673</v>
+        <v>45756</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1495,17 +1495,17 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>47.24</v>
+        <v>44.26</v>
       </c>
       <c r="D27" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E27" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1514,7 +1514,7 @@
     </row>
     <row r="28">
       <c r="A28" s="8" t="n">
-        <v>45756</v>
+        <v>45822</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1522,17 +1522,17 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>44.26</v>
+        <v>47.76</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1541,7 +1541,7 @@
     </row>
     <row r="29">
       <c r="A29" s="8" t="n">
-        <v>45822</v>
+        <v>45827</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1549,17 +1549,17 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>47.76</v>
+        <v>51.37</v>
       </c>
       <c r="D29" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E29" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1568,7 +1568,7 @@
     </row>
     <row r="30">
       <c r="A30" s="8" t="n">
-        <v>45827</v>
+        <v>45829</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1576,17 +1576,17 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>51.37</v>
+        <v>54.71</v>
       </c>
       <c r="D30" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E30" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1595,7 +1595,7 @@
     </row>
     <row r="31">
       <c r="A31" s="8" t="n">
-        <v>45829</v>
+        <v>45834</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1603,17 +1603,17 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>54.71</v>
+        <v>49.06</v>
       </c>
       <c r="D31" t="n">
-        <v>0.06501849328401788</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="E31" t="n">
-        <v>0.06501849328401788</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -1694,7 +1694,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1757,7 +1757,7 @@
     </row>
     <row r="37">
       <c r="A37" s="8" t="n">
-        <v>45784</v>
+        <v>45834</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1765,17 +1765,17 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>44.2</v>
+        <v>49.06</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.05089113162980452</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.05089113162980452</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1784,7 +1784,7 @@
     </row>
     <row r="38">
       <c r="A38" s="8" t="n">
-        <v>45822</v>
+        <v>45673</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1792,17 +1792,17 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>47.76</v>
+        <v>47.24</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0805429864253393</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0805429864253393</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1811,7 +1811,7 @@
     </row>
     <row r="39">
       <c r="A39" s="8" t="n">
-        <v>45827</v>
+        <v>45756</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1819,17 +1819,17 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>51.37</v>
+        <v>44.26</v>
       </c>
       <c r="D39" t="n">
-        <v>0.07558626465661633</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E39" t="n">
-        <v>0.07558626465661633</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1838,7 +1838,7 @@
     </row>
     <row r="40">
       <c r="A40" s="8" t="n">
-        <v>45829</v>
+        <v>45822</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1846,17 +1846,17 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>54.71</v>
+        <v>47.76</v>
       </c>
       <c r="D40" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E40" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1865,7 +1865,7 @@
     </row>
     <row r="41">
       <c r="A41" s="8" t="n">
-        <v>45673</v>
+        <v>45827</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1873,17 +1873,17 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>47.24</v>
+        <v>51.37</v>
       </c>
       <c r="D41" t="n">
-        <v>0.05587840858292359</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E41" t="n">
-        <v>0.05587840858292359</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -1892,7 +1892,7 @@
     </row>
     <row r="42">
       <c r="A42" s="8" t="n">
-        <v>45756</v>
+        <v>45829</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1900,17 +1900,17 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>44.26</v>
+        <v>54.71</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -1919,7 +1919,7 @@
     </row>
     <row r="43">
       <c r="A43" s="8" t="n">
-        <v>45822</v>
+        <v>45834</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1927,17 +1927,17 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>47.76</v>
+        <v>49.06</v>
       </c>
       <c r="D43" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="E43" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -1946,7 +1946,7 @@
     </row>
     <row r="44">
       <c r="A44" s="8" t="n">
-        <v>45827</v>
+        <v>45784</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1954,17 +1954,17 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>51.37</v>
+        <v>44.2</v>
       </c>
       <c r="D44" t="n">
-        <v>0.07558626465661633</v>
+        <v>-0.05089113162980452</v>
       </c>
       <c r="E44" t="n">
-        <v>0.07558626465661633</v>
+        <v>-0.05089113162980452</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa İade Toplama</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -1973,28 +1973,271 @@
     </row>
     <row r="45">
       <c r="A45" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0805429864253393</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.0805429864253393</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>51.37</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="8" t="n">
         <v>45829</v>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Motorin UltraForce</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
         <v>54.71</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D47" t="n">
         <v>0.06501849328401788</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E47" t="n">
         <v>0.06501849328401788</v>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="8" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>49.06</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-0.1032717967464815</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-0.1032717967464815</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="8" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>47.24</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="F49" t="inlineStr">
         <is>
           <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
         </is>
       </c>
-      <c r="G45" t="n">
+      <c r="G49" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="8" t="n">
+        <v>45756</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>44.26</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>51.37</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>54.71</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="8" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>49.06</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-0.1032717967464815</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.1032717967464815</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -2042,7 +2285,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-24</t>
+          <t>2025-06-26</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2059,7 +2302,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-24</t>
+          <t>2025-06-26</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2076,7 +2319,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-24</t>
+          <t>2025-06-26</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2093,7 +2336,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-24</t>
+          <t>2025-06-26</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2110,7 +2353,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-24</t>
+          <t>2025-06-26</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2127,7 +2370,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-24</t>
+          <t>2025-06-26</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2147,7 +2390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4718,6 +4961,19 @@
       </c>
       <c r="C197" t="n">
         <v>53.05</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="8" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>49.06</v>
       </c>
     </row>
   </sheetData>
@@ -4731,7 +4987,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7302,6 +7558,19 @@
       </c>
       <c r="C197" t="n">
         <v>55.3</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="8" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>51.31</v>
       </c>
     </row>
   </sheetData>
@@ -7315,7 +7584,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9886,6 +10155,19 @@
       </c>
       <c r="C197" t="n">
         <v>54.25</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="8" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>50.26</v>
       </c>
     </row>
   </sheetData>
@@ -9899,7 +10181,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12470,6 +12752,19 @@
       </c>
       <c r="C197" t="n">
         <v>54.53</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="8" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>50.54</v>
       </c>
     </row>
   </sheetData>
@@ -12483,7 +12778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15054,6 +15349,19 @@
       </c>
       <c r="C197" t="n">
         <v>55.25</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="8" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>51.26</v>
       </c>
     </row>
   </sheetData>
@@ -15067,7 +15375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17638,6 +17946,19 @@
       </c>
       <c r="C197" t="n">
         <v>54.93</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="8" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>50.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-06-28 02:29:56
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-26</t>
+          <t>2025-06-28</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2302,7 +2302,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-26</t>
+          <t>2025-06-28</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-26</t>
+          <t>2025-06-28</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-26</t>
+          <t>2025-06-28</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-26</t>
+          <t>2025-06-28</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-26</t>
+          <t>2025-06-28</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2390,7 +2390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4974,6 +4974,19 @@
       </c>
       <c r="C198" t="n">
         <v>49.06</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="8" t="n">
+        <v>45836</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>50.2</v>
       </c>
     </row>
   </sheetData>
@@ -4987,7 +5000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7571,6 +7584,19 @@
       </c>
       <c r="C198" t="n">
         <v>51.31</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="8" t="n">
+        <v>45836</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>52.45</v>
       </c>
     </row>
   </sheetData>
@@ -7584,7 +7610,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10168,6 +10194,19 @@
       </c>
       <c r="C198" t="n">
         <v>50.26</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="8" t="n">
+        <v>45836</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>51.4</v>
       </c>
     </row>
   </sheetData>
@@ -10181,7 +10220,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12765,6 +12804,19 @@
       </c>
       <c r="C198" t="n">
         <v>50.54</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="8" t="n">
+        <v>45836</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>51.68</v>
       </c>
     </row>
   </sheetData>
@@ -12778,7 +12830,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15362,6 +15414,19 @@
       </c>
       <c r="C198" t="n">
         <v>51.26</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="8" t="n">
+        <v>45836</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>52.4</v>
       </c>
     </row>
   </sheetData>
@@ -15375,7 +15440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C198"/>
+  <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17959,6 +18024,19 @@
       </c>
       <c r="C198" t="n">
         <v>50.94</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="8" t="n">
+        <v>45836</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>52.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-02 02:42:39
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-28</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2302,7 +2302,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-28</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-28</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-28</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-28</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-28</t>
+          <t>2025-07-02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2390,7 +2390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4987,6 +4987,19 @@
       </c>
       <c r="C199" t="n">
         <v>50.2</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="8" t="n">
+        <v>45840</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>50.22</v>
       </c>
     </row>
   </sheetData>
@@ -5000,7 +5013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7597,6 +7610,19 @@
       </c>
       <c r="C199" t="n">
         <v>52.45</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="8" t="n">
+        <v>45840</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>52.47</v>
       </c>
     </row>
   </sheetData>
@@ -7610,7 +7636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10207,6 +10233,19 @@
       </c>
       <c r="C199" t="n">
         <v>51.4</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="8" t="n">
+        <v>45840</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>51.42</v>
       </c>
     </row>
   </sheetData>
@@ -10220,7 +10259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12817,6 +12856,19 @@
       </c>
       <c r="C199" t="n">
         <v>51.68</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="8" t="n">
+        <v>45840</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>51.7</v>
       </c>
     </row>
   </sheetData>
@@ -12830,7 +12882,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15427,6 +15479,19 @@
       </c>
       <c r="C199" t="n">
         <v>52.4</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="8" t="n">
+        <v>45840</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>52.42</v>
       </c>
     </row>
   </sheetData>
@@ -15440,7 +15505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18037,6 +18102,19 @@
       </c>
       <c r="C199" t="n">
         <v>52.08</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="8" t="n">
+        <v>45840</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>52.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-03 02:44:38
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-03</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2302,7 +2302,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-03</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-03</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-03</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-03</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2025-07-03</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2390,7 +2390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5000,6 +5000,19 @@
       </c>
       <c r="C200" t="n">
         <v>50.22</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>50.26</v>
       </c>
     </row>
   </sheetData>
@@ -5013,7 +5026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7623,6 +7636,19 @@
       </c>
       <c r="C200" t="n">
         <v>52.47</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>52.51</v>
       </c>
     </row>
   </sheetData>
@@ -7636,7 +7662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10246,6 +10272,19 @@
       </c>
       <c r="C200" t="n">
         <v>51.42</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>51.46</v>
       </c>
     </row>
   </sheetData>
@@ -10259,7 +10298,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12869,6 +12908,19 @@
       </c>
       <c r="C200" t="n">
         <v>51.7</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>51.74</v>
       </c>
     </row>
   </sheetData>
@@ -12882,7 +12934,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15492,6 +15544,19 @@
       </c>
       <c r="C200" t="n">
         <v>52.42</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>52.46</v>
       </c>
     </row>
   </sheetData>
@@ -15505,7 +15570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18115,6 +18180,19 @@
       </c>
       <c r="C200" t="n">
         <v>52.1</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>52.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-04 02:42:48
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -765,7 +765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -974,7 +974,7 @@
     </row>
     <row r="8">
       <c r="A8" s="8" t="n">
-        <v>45673</v>
+        <v>45841</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -982,17 +982,17 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>48.88</v>
+        <v>54.57</v>
       </c>
       <c r="D8" t="n">
-        <v>0.05663640293990491</v>
+        <v>0.06457276628950459</v>
       </c>
       <c r="E8" t="n">
-        <v>0.05663640293990491</v>
+        <v>0.06457276628950459</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Servis Kayseri</t>
+          <t>Servis Diyarbakır</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1001,7 +1001,7 @@
     </row>
     <row r="9">
       <c r="A9" s="8" t="n">
-        <v>45756</v>
+        <v>45673</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1009,13 +1009,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>46.03</v>
+        <v>48.88</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.05830605564648117</v>
+        <v>0.05663640293990491</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="10">
       <c r="A10" s="8" t="n">
-        <v>45822</v>
+        <v>45756</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>49.64</v>
+        <v>46.03</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07842711275255265</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="E10" t="n">
-        <v>0.07842711275255265</v>
+        <v>-0.05830605564648117</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="11">
       <c r="A11" s="8" t="n">
-        <v>45827</v>
+        <v>45822</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1063,13 +1063,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>53.25</v>
+        <v>49.64</v>
       </c>
       <c r="D11" t="n">
-        <v>0.07272360999194194</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="E11" t="n">
-        <v>0.07272360999194194</v>
+        <v>0.07842711275255265</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="12">
       <c r="A12" s="8" t="n">
-        <v>45829</v>
+        <v>45827</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1090,13 +1090,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>56.59</v>
+        <v>53.25</v>
       </c>
       <c r="D12" t="n">
-        <v>0.06272300469483572</v>
+        <v>0.07272360999194194</v>
       </c>
       <c r="E12" t="n">
-        <v>0.06272300469483572</v>
+        <v>0.07272360999194194</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="13">
       <c r="A13" s="8" t="n">
-        <v>45834</v>
+        <v>45829</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1117,13 +1117,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>50.94</v>
+        <v>56.59</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.09984096130058329</v>
+        <v>0.06272300469483572</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.09984096130058329</v>
+        <v>0.06272300469483572</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="14">
       <c r="A14" s="8" t="n">
-        <v>45673</v>
+        <v>45834</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1144,17 +1144,17 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>48.57</v>
+        <v>50.94</v>
       </c>
       <c r="D14" t="n">
-        <v>0.05678851174934718</v>
+        <v>-0.09984096130058329</v>
       </c>
       <c r="E14" t="n">
-        <v>0.05678851174934718</v>
+        <v>-0.09984096130058329</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -1163,7 +1163,7 @@
     </row>
     <row r="15">
       <c r="A15" s="8" t="n">
-        <v>45756</v>
+        <v>45841</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1171,17 +1171,17 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>45.66</v>
+        <v>54.26</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.05991352686843743</v>
+        <v>0.06517471535139374</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.05991352686843743</v>
+        <v>0.06517471535139374</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Servis Samsun</t>
+          <t>Servis Kayseri</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1190,7 +1190,7 @@
     </row>
     <row r="16">
       <c r="A16" s="8" t="n">
-        <v>45822</v>
+        <v>45673</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1198,13 +1198,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>49.24</v>
+        <v>48.57</v>
       </c>
       <c r="D16" t="n">
-        <v>0.07840560665790641</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="E16" t="n">
-        <v>0.07840560665790641</v>
+        <v>0.05678851174934718</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="17">
       <c r="A17" s="8" t="n">
-        <v>45827</v>
+        <v>45756</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1225,13 +1225,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>52.85</v>
+        <v>45.66</v>
       </c>
       <c r="D17" t="n">
-        <v>0.07331437855402112</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="E17" t="n">
-        <v>0.07331437855402112</v>
+        <v>-0.05991352686843743</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="18">
       <c r="A18" s="8" t="n">
-        <v>45829</v>
+        <v>45822</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1252,13 +1252,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>56.19</v>
+        <v>49.24</v>
       </c>
       <c r="D18" t="n">
-        <v>0.06319772942289492</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="E18" t="n">
-        <v>0.06319772942289492</v>
+        <v>0.07840560665790641</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="19">
       <c r="A19" s="8" t="n">
-        <v>45834</v>
+        <v>45827</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1279,13 +1279,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>50.54</v>
+        <v>52.85</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.1005516995906744</v>
+        <v>0.07331437855402112</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.1005516995906744</v>
+        <v>0.07331437855402112</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="20">
       <c r="A20" s="8" t="n">
-        <v>45673</v>
+        <v>45829</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1306,17 +1306,17 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>47.24</v>
+        <v>56.19</v>
       </c>
       <c r="D20" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.06319772942289492</v>
       </c>
       <c r="E20" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.06319772942289492</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1325,7 +1325,7 @@
     </row>
     <row r="21">
       <c r="A21" s="8" t="n">
-        <v>45756</v>
+        <v>45834</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1333,17 +1333,17 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>44.26</v>
+        <v>50.54</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.06308213378492811</v>
+        <v>-0.1005516995906744</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.06308213378492811</v>
+        <v>-0.1005516995906744</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1352,7 +1352,7 @@
     </row>
     <row r="22">
       <c r="A22" s="8" t="n">
-        <v>45822</v>
+        <v>45841</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1360,17 +1360,17 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>47.76</v>
+        <v>53.85</v>
       </c>
       <c r="D22" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.06549267906608636</v>
       </c>
       <c r="E22" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.06549267906608636</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Spot Araç Anadolu Toplama</t>
+          <t>Servis Samsun</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1379,7 +1379,7 @@
     </row>
     <row r="23">
       <c r="A23" s="8" t="n">
-        <v>45827</v>
+        <v>45673</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1387,13 +1387,13 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>51.37</v>
+        <v>47.24</v>
       </c>
       <c r="D23" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E23" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="24">
       <c r="A24" s="8" t="n">
-        <v>45829</v>
+        <v>45756</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1414,13 +1414,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>54.71</v>
+        <v>44.26</v>
       </c>
       <c r="D24" t="n">
-        <v>0.06501849328401788</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E24" t="n">
-        <v>0.06501849328401788</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="25">
       <c r="A25" s="8" t="n">
-        <v>45834</v>
+        <v>45822</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1441,13 +1441,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>49.06</v>
+        <v>47.76</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.1032717967464815</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.1032717967464815</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="26">
       <c r="A26" s="8" t="n">
-        <v>45673</v>
+        <v>45827</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1468,17 +1468,17 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>47.24</v>
+        <v>51.37</v>
       </c>
       <c r="D26" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E26" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1487,7 +1487,7 @@
     </row>
     <row r="27">
       <c r="A27" s="8" t="n">
-        <v>45756</v>
+        <v>45829</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1495,17 +1495,17 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>44.26</v>
+        <v>54.71</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1514,7 +1514,7 @@
     </row>
     <row r="28">
       <c r="A28" s="8" t="n">
-        <v>45822</v>
+        <v>45834</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1522,17 +1522,17 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>47.76</v>
+        <v>49.06</v>
       </c>
       <c r="D28" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="E28" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1541,7 +1541,7 @@
     </row>
     <row r="29">
       <c r="A29" s="8" t="n">
-        <v>45827</v>
+        <v>45841</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1549,17 +1549,17 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>51.37</v>
+        <v>52.37</v>
       </c>
       <c r="D29" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.0674684060334283</v>
       </c>
       <c r="E29" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.0674684060334283</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Spot Araç Avrupa&amp;Anadolu</t>
+          <t>Spot Araç Anadolu Toplama</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1568,7 +1568,7 @@
     </row>
     <row r="30">
       <c r="A30" s="8" t="n">
-        <v>45829</v>
+        <v>45673</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1576,13 +1576,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>54.71</v>
+        <v>47.24</v>
       </c>
       <c r="D30" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E30" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="31">
       <c r="A31" s="8" t="n">
-        <v>45834</v>
+        <v>45756</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1603,13 +1603,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>49.06</v>
+        <v>44.26</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.1032717967464815</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.1032717967464815</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="32">
       <c r="A32" s="8" t="n">
-        <v>45673</v>
+        <v>45822</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1630,17 +1630,17 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>47.24</v>
+        <v>47.76</v>
       </c>
       <c r="D32" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E32" t="n">
-        <v>0.07023108291798819</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -1649,7 +1649,7 @@
     </row>
     <row r="33">
       <c r="A33" s="8" t="n">
-        <v>45756</v>
+        <v>45827</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1657,17 +1657,17 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>44.26</v>
+        <v>51.37</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -1676,7 +1676,7 @@
     </row>
     <row r="34">
       <c r="A34" s="8" t="n">
-        <v>45822</v>
+        <v>45829</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1684,17 +1684,17 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>47.76</v>
+        <v>54.71</v>
       </c>
       <c r="D34" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E34" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1703,7 +1703,7 @@
     </row>
     <row r="35">
       <c r="A35" s="8" t="n">
-        <v>45827</v>
+        <v>45834</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1711,17 +1711,17 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>51.37</v>
+        <v>49.06</v>
       </c>
       <c r="D35" t="n">
-        <v>0.07558626465661633</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="E35" t="n">
-        <v>0.07558626465661633</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1730,7 +1730,7 @@
     </row>
     <row r="36">
       <c r="A36" s="8" t="n">
-        <v>45829</v>
+        <v>45841</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1738,17 +1738,17 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>54.71</v>
+        <v>52.37</v>
       </c>
       <c r="D36" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.0674684060334283</v>
       </c>
       <c r="E36" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.0674684060334283</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Spot Araç Teknosa</t>
+          <t>Spot Araç Avrupa&amp;Anadolu</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1757,7 +1757,7 @@
     </row>
     <row r="37">
       <c r="A37" s="8" t="n">
-        <v>45834</v>
+        <v>45673</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1765,13 +1765,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>49.06</v>
+        <v>47.24</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.1032717967464815</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.1032717967464815</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="38">
       <c r="A38" s="8" t="n">
-        <v>45673</v>
+        <v>45756</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1792,17 +1792,17 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>47.24</v>
+        <v>44.26</v>
       </c>
       <c r="D38" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E38" t="n">
-        <v>0.07023108291798819</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1811,7 +1811,7 @@
     </row>
     <row r="39">
       <c r="A39" s="8" t="n">
-        <v>45756</v>
+        <v>45822</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1819,17 +1819,17 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>44.26</v>
+        <v>47.76</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1838,7 +1838,7 @@
     </row>
     <row r="40">
       <c r="A40" s="8" t="n">
-        <v>45822</v>
+        <v>45827</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1846,17 +1846,17 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>47.76</v>
+        <v>51.37</v>
       </c>
       <c r="D40" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E40" t="n">
-        <v>0.07907817442385912</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1865,7 +1865,7 @@
     </row>
     <row r="41">
       <c r="A41" s="8" t="n">
-        <v>45827</v>
+        <v>45829</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1873,17 +1873,17 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>51.37</v>
+        <v>54.71</v>
       </c>
       <c r="D41" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E41" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -1892,7 +1892,7 @@
     </row>
     <row r="42">
       <c r="A42" s="8" t="n">
-        <v>45829</v>
+        <v>45834</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1900,17 +1900,17 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>54.71</v>
+        <v>49.06</v>
       </c>
       <c r="D42" t="n">
-        <v>0.06501849328401788</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="E42" t="n">
-        <v>0.06501849328401788</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -1919,7 +1919,7 @@
     </row>
     <row r="43">
       <c r="A43" s="8" t="n">
-        <v>45834</v>
+        <v>45841</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1927,17 +1927,17 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>49.06</v>
+        <v>52.37</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.1032717967464815</v>
+        <v>0.0674684060334283</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.1032717967464815</v>
+        <v>0.0674684060334283</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa Toplama</t>
+          <t>Spot Araç Teknosa</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -1946,7 +1946,7 @@
     </row>
     <row r="44">
       <c r="A44" s="8" t="n">
-        <v>45784</v>
+        <v>45673</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1954,17 +1954,17 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44.2</v>
+        <v>47.24</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.05089113162980452</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.05089113162980452</v>
+        <v>0.07023108291798819</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -1973,7 +1973,7 @@
     </row>
     <row r="45">
       <c r="A45" s="8" t="n">
-        <v>45822</v>
+        <v>45756</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1981,17 +1981,17 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>47.76</v>
+        <v>44.26</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0805429864253393</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="E45" t="n">
-        <v>0.0805429864253393</v>
+        <v>-0.06308213378492811</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -2000,7 +2000,7 @@
     </row>
     <row r="46">
       <c r="A46" s="8" t="n">
-        <v>45827</v>
+        <v>45822</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -2008,17 +2008,17 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>51.37</v>
+        <v>47.76</v>
       </c>
       <c r="D46" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="E46" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.07907817442385912</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -2027,7 +2027,7 @@
     </row>
     <row r="47">
       <c r="A47" s="8" t="n">
-        <v>45829</v>
+        <v>45827</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -2035,17 +2035,17 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>54.71</v>
+        <v>51.37</v>
       </c>
       <c r="D47" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E47" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -2054,7 +2054,7 @@
     </row>
     <row r="48">
       <c r="A48" s="8" t="n">
-        <v>45834</v>
+        <v>45829</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -2062,17 +2062,17 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>49.06</v>
+        <v>54.71</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.1032717967464815</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.1032717967464815</v>
+        <v>0.06501849328401788</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa İade Toplama</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2081,7 +2081,7 @@
     </row>
     <row r="49">
       <c r="A49" s="8" t="n">
-        <v>45673</v>
+        <v>45834</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -2089,17 +2089,17 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>47.24</v>
+        <v>49.06</v>
       </c>
       <c r="D49" t="n">
-        <v>0.05587840858292359</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="E49" t="n">
-        <v>0.05587840858292359</v>
+        <v>-0.1032717967464815</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -2108,7 +2108,7 @@
     </row>
     <row r="50">
       <c r="A50" s="8" t="n">
-        <v>45756</v>
+        <v>45841</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -2116,17 +2116,17 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>44.26</v>
+        <v>52.37</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.0674684060334283</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.06308213378492811</v>
+        <v>0.0674684060334283</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa Toplama</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2135,7 +2135,7 @@
     </row>
     <row r="51">
       <c r="A51" s="8" t="n">
-        <v>45822</v>
+        <v>45784</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -2143,17 +2143,17 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>47.76</v>
+        <v>44.2</v>
       </c>
       <c r="D51" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.05089113162980452</v>
       </c>
       <c r="E51" t="n">
-        <v>0.07907817442385912</v>
+        <v>-0.05089113162980452</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa İade Toplama</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -2162,7 +2162,7 @@
     </row>
     <row r="52">
       <c r="A52" s="8" t="n">
-        <v>45827</v>
+        <v>45822</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -2170,17 +2170,17 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>51.37</v>
+        <v>47.76</v>
       </c>
       <c r="D52" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.0805429864253393</v>
       </c>
       <c r="E52" t="n">
-        <v>0.07558626465661633</v>
+        <v>0.0805429864253393</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa İade Toplama</t>
         </is>
       </c>
       <c r="G52" t="n">
@@ -2189,7 +2189,7 @@
     </row>
     <row r="53">
       <c r="A53" s="8" t="n">
-        <v>45829</v>
+        <v>45827</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -2197,17 +2197,17 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>54.71</v>
+        <v>51.37</v>
       </c>
       <c r="D53" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="E53" t="n">
-        <v>0.06501849328401788</v>
+        <v>0.07558626465661633</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+          <t>TL/Desi Avrupa İade Toplama</t>
         </is>
       </c>
       <c r="G53" t="n">
@@ -2216,28 +2216,271 @@
     </row>
     <row r="54">
       <c r="A54" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>54.71</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="8" t="n">
         <v>45834</v>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Motorin UltraForce</t>
-        </is>
-      </c>
-      <c r="C54" t="n">
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
         <v>49.06</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D55" t="n">
         <v>-0.1032717967464815</v>
       </c>
-      <c r="E54" t="n">
+      <c r="E55" t="n">
         <v>-0.1032717967464815</v>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>52.37</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.0674684060334283</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.0674684060334283</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa İade Toplama</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="8" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>47.24</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.05587840858292359</v>
+      </c>
+      <c r="F57" t="inlineStr">
         <is>
           <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
         </is>
       </c>
-      <c r="G54" t="n">
+      <c r="G57" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="8" t="n">
+        <v>45756</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>44.26</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-0.06308213378492811</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="8" t="n">
+        <v>45822</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>47.76</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.07907817442385912</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="8" t="n">
+        <v>45827</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>51.37</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.07558626465661633</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="8" t="n">
+        <v>45829</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>54.71</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.06501849328401788</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="8" t="n">
+        <v>45834</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>49.06</v>
+      </c>
+      <c r="D62" t="n">
+        <v>-0.1032717967464815</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-0.1032717967464815</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>52.37</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.0674684060334283</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.0674684060334283</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>TL/Desi Avrupa&amp;Anadolu Dağıtım</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -2390,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:C202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5013,6 +5256,19 @@
       </c>
       <c r="C201" t="n">
         <v>50.26</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>52.37</v>
       </c>
     </row>
   </sheetData>
@@ -5026,7 +5282,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:C202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7649,6 +7905,19 @@
       </c>
       <c r="C201" t="n">
         <v>52.51</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>54.62</v>
       </c>
     </row>
   </sheetData>
@@ -7662,7 +7931,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:C202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10285,6 +10554,19 @@
       </c>
       <c r="C201" t="n">
         <v>51.46</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>53.57</v>
       </c>
     </row>
   </sheetData>
@@ -10298,7 +10580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:C202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12921,6 +13203,19 @@
       </c>
       <c r="C201" t="n">
         <v>51.74</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>53.85</v>
       </c>
     </row>
   </sheetData>
@@ -12934,7 +13229,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:C202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15557,6 +15852,19 @@
       </c>
       <c r="C201" t="n">
         <v>52.46</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>54.57</v>
       </c>
     </row>
   </sheetData>
@@ -15570,7 +15878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:C202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18193,6 +18501,19 @@
       </c>
       <c r="C201" t="n">
         <v>52.15</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="8" t="n">
+        <v>45841</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>54.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-05 02:29:27
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-03</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-03</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-03</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-03</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-03</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-03</t>
+          <t>2025-07-05</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C202"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5268,6 +5268,19 @@
         </is>
       </c>
       <c r="C202" t="n">
+        <v>52.37</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="8" t="n">
+        <v>45843</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
         <v>52.37</v>
       </c>
     </row>
@@ -5282,7 +5295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C202"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7917,6 +7930,19 @@
         </is>
       </c>
       <c r="C202" t="n">
+        <v>54.62</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="8" t="n">
+        <v>45843</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
         <v>54.62</v>
       </c>
     </row>
@@ -7931,7 +7957,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C202"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10566,6 +10592,19 @@
         </is>
       </c>
       <c r="C202" t="n">
+        <v>53.57</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="8" t="n">
+        <v>45843</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
         <v>53.57</v>
       </c>
     </row>
@@ -10580,7 +10619,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C202"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13215,6 +13254,19 @@
         </is>
       </c>
       <c r="C202" t="n">
+        <v>53.85</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="8" t="n">
+        <v>45843</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
         <v>53.85</v>
       </c>
     </row>
@@ -13229,7 +13281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C202"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15864,6 +15916,19 @@
         </is>
       </c>
       <c r="C202" t="n">
+        <v>54.57</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="8" t="n">
+        <v>45843</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
         <v>54.57</v>
       </c>
     </row>
@@ -15878,7 +15943,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C202"/>
+  <dimension ref="A1:C203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18513,6 +18578,19 @@
         </is>
       </c>
       <c r="C202" t="n">
+        <v>54.26</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="8" t="n">
+        <v>45843</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
         <v>54.26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-08 02:44:10
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-07-08</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-07-08</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-07-08</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-07-08</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-07-08</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-05</t>
+          <t>2025-07-08</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C203"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5282,6 +5282,19 @@
       </c>
       <c r="C203" t="n">
         <v>52.37</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="8" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>52.41</v>
       </c>
     </row>
   </sheetData>
@@ -5295,7 +5308,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C203"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7944,6 +7957,19 @@
       </c>
       <c r="C203" t="n">
         <v>54.62</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="8" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>54.67</v>
       </c>
     </row>
   </sheetData>
@@ -7957,7 +7983,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C203"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10606,6 +10632,19 @@
       </c>
       <c r="C203" t="n">
         <v>53.57</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="8" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>53.62</v>
       </c>
     </row>
   </sheetData>
@@ -10619,7 +10658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C203"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13268,6 +13307,19 @@
       </c>
       <c r="C203" t="n">
         <v>53.85</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="8" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>53.9</v>
       </c>
     </row>
   </sheetData>
@@ -13281,7 +13333,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C203"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15930,6 +15982,19 @@
       </c>
       <c r="C203" t="n">
         <v>54.57</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="8" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>54.62</v>
       </c>
     </row>
   </sheetData>
@@ -15943,7 +16008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C203"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18592,6 +18657,19 @@
       </c>
       <c r="C203" t="n">
         <v>54.26</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="8" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>54.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-09 02:46:11
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-08</t>
+          <t>2025-07-09</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-08</t>
+          <t>2025-07-09</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-08</t>
+          <t>2025-07-09</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-08</t>
+          <t>2025-07-09</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-08</t>
+          <t>2025-07-09</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-08</t>
+          <t>2025-07-09</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5295,6 +5295,19 @@
       </c>
       <c r="C204" t="n">
         <v>52.41</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="8" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>53.56</v>
       </c>
     </row>
   </sheetData>
@@ -5308,7 +5321,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7970,6 +7983,19 @@
       </c>
       <c r="C204" t="n">
         <v>54.67</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="8" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>55.82</v>
       </c>
     </row>
   </sheetData>
@@ -7983,7 +8009,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10645,6 +10671,19 @@
       </c>
       <c r="C204" t="n">
         <v>53.62</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="8" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>54.77</v>
       </c>
     </row>
   </sheetData>
@@ -10658,7 +10697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13320,6 +13359,19 @@
       </c>
       <c r="C204" t="n">
         <v>53.9</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="8" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>55.05</v>
       </c>
     </row>
   </sheetData>
@@ -13333,7 +13385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15995,6 +16047,19 @@
       </c>
       <c r="C204" t="n">
         <v>54.62</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="8" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>55.77</v>
       </c>
     </row>
   </sheetData>
@@ -16008,7 +16073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C204"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18670,6 +18735,19 @@
       </c>
       <c r="C204" t="n">
         <v>54.31</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="8" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>55.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-12 02:49:13
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-07-12</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-07-12</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-07-12</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-07-12</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-07-12</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-09</t>
+          <t>2025-07-12</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:C206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5308,6 +5308,19 @@
       </c>
       <c r="C205" t="n">
         <v>53.56</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="8" t="n">
+        <v>45850</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>53.61</v>
       </c>
     </row>
   </sheetData>
@@ -5321,7 +5334,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:C206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7996,6 +8009,19 @@
       </c>
       <c r="C205" t="n">
         <v>55.82</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="8" t="n">
+        <v>45850</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>55.87</v>
       </c>
     </row>
   </sheetData>
@@ -8009,7 +8035,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:C206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10684,6 +10710,19 @@
       </c>
       <c r="C205" t="n">
         <v>54.77</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="8" t="n">
+        <v>45850</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>54.82</v>
       </c>
     </row>
   </sheetData>
@@ -10697,7 +10736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:C206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13372,6 +13411,19 @@
       </c>
       <c r="C205" t="n">
         <v>55.05</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="8" t="n">
+        <v>45850</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>55.1</v>
       </c>
     </row>
   </sheetData>
@@ -13385,7 +13437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:C206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16060,6 +16112,19 @@
       </c>
       <c r="C205" t="n">
         <v>55.77</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="8" t="n">
+        <v>45850</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>55.82</v>
       </c>
     </row>
   </sheetData>
@@ -16073,7 +16138,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C205"/>
+  <dimension ref="A1:C206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18748,6 +18813,19 @@
       </c>
       <c r="C205" t="n">
         <v>55.46</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="8" t="n">
+        <v>45850</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>55.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-19 02:45:13
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-12</t>
+          <t>2025-07-19</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-12</t>
+          <t>2025-07-19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-12</t>
+          <t>2025-07-19</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-12</t>
+          <t>2025-07-19</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-12</t>
+          <t>2025-07-19</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-12</t>
+          <t>2025-07-19</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C206"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5320,6 +5320,19 @@
         </is>
       </c>
       <c r="C206" t="n">
+        <v>53.61</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="8" t="n">
+        <v>45857</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
         <v>53.61</v>
       </c>
     </row>
@@ -5334,7 +5347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C206"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8022,6 +8035,19 @@
       </c>
       <c r="C206" t="n">
         <v>55.87</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="8" t="n">
+        <v>45857</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>55.9</v>
       </c>
     </row>
   </sheetData>
@@ -8035,7 +8061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C206"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10723,6 +10749,19 @@
       </c>
       <c r="C206" t="n">
         <v>54.82</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="8" t="n">
+        <v>45857</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>54.85</v>
       </c>
     </row>
   </sheetData>
@@ -10736,7 +10775,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C206"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13424,6 +13463,19 @@
       </c>
       <c r="C206" t="n">
         <v>55.1</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="8" t="n">
+        <v>45857</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>55.13</v>
       </c>
     </row>
   </sheetData>
@@ -13437,7 +13489,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C206"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16125,6 +16177,19 @@
       </c>
       <c r="C206" t="n">
         <v>55.82</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="8" t="n">
+        <v>45857</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>55.85</v>
       </c>
     </row>
   </sheetData>
@@ -16138,7 +16203,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C206"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18826,6 +18891,19 @@
       </c>
       <c r="C206" t="n">
         <v>55.51</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="8" t="n">
+        <v>45857</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>55.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-23 02:53:42
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-19</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-19</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-19</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-19</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-19</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-19</t>
+          <t>2025-07-23</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5334,6 +5334,19 @@
       </c>
       <c r="C207" t="n">
         <v>53.61</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="8" t="n">
+        <v>45861</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>53.67</v>
       </c>
     </row>
   </sheetData>
@@ -5347,7 +5360,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8048,6 +8061,19 @@
       </c>
       <c r="C207" t="n">
         <v>55.9</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="8" t="n">
+        <v>45861</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>55.96</v>
       </c>
     </row>
   </sheetData>
@@ -8061,7 +8087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10762,6 +10788,19 @@
       </c>
       <c r="C207" t="n">
         <v>54.85</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="8" t="n">
+        <v>45861</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>54.91</v>
       </c>
     </row>
   </sheetData>
@@ -10775,7 +10814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13476,6 +13515,19 @@
       </c>
       <c r="C207" t="n">
         <v>55.13</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="8" t="n">
+        <v>45861</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>55.19</v>
       </c>
     </row>
   </sheetData>
@@ -13489,7 +13541,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16190,6 +16242,19 @@
       </c>
       <c r="C207" t="n">
         <v>55.85</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="8" t="n">
+        <v>45861</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>55.91</v>
       </c>
     </row>
   </sheetData>
@@ -16203,7 +16268,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18904,6 +18969,19 @@
       </c>
       <c r="C207" t="n">
         <v>55.54</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="8" t="n">
+        <v>45861</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>55.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-24 02:52:25
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-23</t>
+          <t>2025-07-24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-23</t>
+          <t>2025-07-24</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-23</t>
+          <t>2025-07-24</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-23</t>
+          <t>2025-07-24</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-23</t>
+          <t>2025-07-24</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-23</t>
+          <t>2025-07-24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C208"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5346,6 +5346,19 @@
         </is>
       </c>
       <c r="C208" t="n">
+        <v>53.67</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="8" t="n">
+        <v>45862</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
         <v>53.67</v>
       </c>
     </row>
@@ -5360,7 +5373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C208"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8073,6 +8086,19 @@
         </is>
       </c>
       <c r="C208" t="n">
+        <v>55.96</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="8" t="n">
+        <v>45862</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
         <v>55.96</v>
       </c>
     </row>
@@ -8087,7 +8113,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C208"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10800,6 +10826,19 @@
         </is>
       </c>
       <c r="C208" t="n">
+        <v>54.91</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="8" t="n">
+        <v>45862</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
         <v>54.91</v>
       </c>
     </row>
@@ -10814,7 +10853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C208"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13527,6 +13566,19 @@
         </is>
       </c>
       <c r="C208" t="n">
+        <v>55.19</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="8" t="n">
+        <v>45862</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
         <v>55.19</v>
       </c>
     </row>
@@ -13541,7 +13593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C208"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16254,6 +16306,19 @@
         </is>
       </c>
       <c r="C208" t="n">
+        <v>55.91</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="8" t="n">
+        <v>45862</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
         <v>55.91</v>
       </c>
     </row>
@@ -16268,7 +16333,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C208"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18981,6 +19046,19 @@
         </is>
       </c>
       <c r="C208" t="n">
+        <v>55.6</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="8" t="n">
+        <v>45862</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
         <v>55.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-07-29 03:03:56
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-24</t>
+          <t>2025-07-29</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C209"/>
+  <dimension ref="A1:C210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5360,6 +5360,19 @@
       </c>
       <c r="C209" t="n">
         <v>53.67</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="8" t="n">
+        <v>45867</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>53.7</v>
       </c>
     </row>
   </sheetData>
@@ -5373,7 +5386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C209"/>
+  <dimension ref="A1:C210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8100,6 +8113,19 @@
       </c>
       <c r="C209" t="n">
         <v>55.96</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="8" t="n">
+        <v>45867</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>55.99</v>
       </c>
     </row>
   </sheetData>
@@ -8113,7 +8139,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C209"/>
+  <dimension ref="A1:C210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10840,6 +10866,19 @@
       </c>
       <c r="C209" t="n">
         <v>54.91</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="8" t="n">
+        <v>45867</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>54.94</v>
       </c>
     </row>
   </sheetData>
@@ -10853,7 +10892,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C209"/>
+  <dimension ref="A1:C210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13580,6 +13619,19 @@
       </c>
       <c r="C209" t="n">
         <v>55.19</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="8" t="n">
+        <v>45867</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>55.22</v>
       </c>
     </row>
   </sheetData>
@@ -13593,7 +13645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C209"/>
+  <dimension ref="A1:C210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16320,6 +16372,19 @@
       </c>
       <c r="C209" t="n">
         <v>55.91</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="8" t="n">
+        <v>45867</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>55.94</v>
       </c>
     </row>
   </sheetData>
@@ -16333,7 +16398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C209"/>
+  <dimension ref="A1:C210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19060,6 +19125,19 @@
       </c>
       <c r="C209" t="n">
         <v>55.6</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="8" t="n">
+        <v>45867</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>55.63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-02 02:48:07
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-07-29</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C210"/>
+  <dimension ref="A1:C211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5373,6 +5373,19 @@
       </c>
       <c r="C210" t="n">
         <v>53.7</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="8" t="n">
+        <v>45871</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>53.76</v>
       </c>
     </row>
   </sheetData>
@@ -5386,7 +5399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C210"/>
+  <dimension ref="A1:C211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8126,6 +8139,19 @@
       </c>
       <c r="C210" t="n">
         <v>55.99</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="8" t="n">
+        <v>45871</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>56.05</v>
       </c>
     </row>
   </sheetData>
@@ -8139,7 +8165,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C210"/>
+  <dimension ref="A1:C211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10879,6 +10905,19 @@
       </c>
       <c r="C210" t="n">
         <v>54.94</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="8" t="n">
+        <v>45871</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -10892,7 +10931,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C210"/>
+  <dimension ref="A1:C211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13632,6 +13671,19 @@
       </c>
       <c r="C210" t="n">
         <v>55.22</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="8" t="n">
+        <v>45871</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>55.28</v>
       </c>
     </row>
   </sheetData>
@@ -13645,7 +13697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C210"/>
+  <dimension ref="A1:C211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16385,6 +16437,19 @@
       </c>
       <c r="C210" t="n">
         <v>55.94</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="8" t="n">
+        <v>45871</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -16398,7 +16463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C210"/>
+  <dimension ref="A1:C211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19138,6 +19203,19 @@
       </c>
       <c r="C210" t="n">
         <v>55.63</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="8" t="n">
+        <v>45871</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>55.69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-07 02:57:54
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-08-07</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-08-07</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-08-07</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-08-07</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-08-07</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-08-07</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C211"/>
+  <dimension ref="A1:C212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5386,6 +5386,19 @@
       </c>
       <c r="C211" t="n">
         <v>53.76</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="8" t="n">
+        <v>45876</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>52.05</v>
       </c>
     </row>
   </sheetData>
@@ -5399,7 +5412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C211"/>
+  <dimension ref="A1:C212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8152,6 +8165,19 @@
       </c>
       <c r="C211" t="n">
         <v>56.05</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="8" t="n">
+        <v>45876</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>54.34</v>
       </c>
     </row>
   </sheetData>
@@ -8165,7 +8191,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C211"/>
+  <dimension ref="A1:C212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10918,6 +10944,19 @@
       </c>
       <c r="C211" t="n">
         <v>55</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="8" t="n">
+        <v>45876</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>53.29</v>
       </c>
     </row>
   </sheetData>
@@ -10931,7 +10970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C211"/>
+  <dimension ref="A1:C212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13684,6 +13723,19 @@
       </c>
       <c r="C211" t="n">
         <v>55.28</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="8" t="n">
+        <v>45876</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>53.57</v>
       </c>
     </row>
   </sheetData>
@@ -13697,7 +13749,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C211"/>
+  <dimension ref="A1:C212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16450,6 +16502,19 @@
       </c>
       <c r="C211" t="n">
         <v>56</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="8" t="n">
+        <v>45876</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>54.29</v>
       </c>
     </row>
   </sheetData>
@@ -16463,7 +16528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C211"/>
+  <dimension ref="A1:C212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19216,6 +19281,19 @@
       </c>
       <c r="C211" t="n">
         <v>55.69</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="8" t="n">
+        <v>45876</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>53.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-09 02:43:05
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-07</t>
+          <t>2025-08-09</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-07</t>
+          <t>2025-08-09</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-07</t>
+          <t>2025-08-09</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-07</t>
+          <t>2025-08-09</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-07</t>
+          <t>2025-08-09</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-07</t>
+          <t>2025-08-09</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5398,6 +5398,19 @@
         </is>
       </c>
       <c r="C212" t="n">
+        <v>52.05</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="8" t="n">
+        <v>45878</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
         <v>52.05</v>
       </c>
     </row>
@@ -5412,7 +5425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8177,6 +8190,19 @@
         </is>
       </c>
       <c r="C212" t="n">
+        <v>54.34</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="8" t="n">
+        <v>45878</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
         <v>54.34</v>
       </c>
     </row>
@@ -8191,7 +8217,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10956,6 +10982,19 @@
         </is>
       </c>
       <c r="C212" t="n">
+        <v>53.29</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="8" t="n">
+        <v>45878</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
         <v>53.29</v>
       </c>
     </row>
@@ -10970,7 +11009,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13735,6 +13774,19 @@
         </is>
       </c>
       <c r="C212" t="n">
+        <v>53.57</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="8" t="n">
+        <v>45878</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
         <v>53.57</v>
       </c>
     </row>
@@ -13749,7 +13801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16514,6 +16566,19 @@
         </is>
       </c>
       <c r="C212" t="n">
+        <v>54.29</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="8" t="n">
+        <v>45878</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
         <v>54.29</v>
       </c>
     </row>
@@ -16528,7 +16593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19293,6 +19358,19 @@
         </is>
       </c>
       <c r="C212" t="n">
+        <v>53.98</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="8" t="n">
+        <v>45878</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
         <v>53.98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-13 02:43:49
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-09</t>
+          <t>2025-08-13</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-09</t>
+          <t>2025-08-13</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-09</t>
+          <t>2025-08-13</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-09</t>
+          <t>2025-08-13</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-09</t>
+          <t>2025-08-13</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-09</t>
+          <t>2025-08-13</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C213"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5412,6 +5412,19 @@
       </c>
       <c r="C213" t="n">
         <v>52.05</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="8" t="n">
+        <v>45882</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>52.08</v>
       </c>
     </row>
   </sheetData>
@@ -5425,7 +5438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C213"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8204,6 +8217,19 @@
       </c>
       <c r="C213" t="n">
         <v>54.34</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="8" t="n">
+        <v>45882</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>54.39</v>
       </c>
     </row>
   </sheetData>
@@ -8217,7 +8243,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C213"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10996,6 +11022,19 @@
       </c>
       <c r="C213" t="n">
         <v>53.29</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="8" t="n">
+        <v>45882</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>53.33</v>
       </c>
     </row>
   </sheetData>
@@ -11009,7 +11048,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C213"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13788,6 +13827,19 @@
       </c>
       <c r="C213" t="n">
         <v>53.57</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="8" t="n">
+        <v>45882</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>53.61</v>
       </c>
     </row>
   </sheetData>
@@ -13801,7 +13853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C213"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16580,6 +16632,19 @@
       </c>
       <c r="C213" t="n">
         <v>54.29</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="8" t="n">
+        <v>45882</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>54.34</v>
       </c>
     </row>
   </sheetData>
@@ -16593,7 +16658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C213"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19372,6 +19437,19 @@
       </c>
       <c r="C213" t="n">
         <v>53.98</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="8" t="n">
+        <v>45882</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>54.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-16 02:29:23
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-13</t>
+          <t>2025-08-16</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-13</t>
+          <t>2025-08-16</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-13</t>
+          <t>2025-08-16</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-13</t>
+          <t>2025-08-16</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-13</t>
+          <t>2025-08-16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-13</t>
+          <t>2025-08-16</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5425,6 +5425,19 @@
       </c>
       <c r="C214" t="n">
         <v>52.08</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="8" t="n">
+        <v>45885</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>52.11</v>
       </c>
     </row>
   </sheetData>
@@ -5438,7 +5451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8230,6 +8243,19 @@
       </c>
       <c r="C214" t="n">
         <v>54.39</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="8" t="n">
+        <v>45885</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>54.43</v>
       </c>
     </row>
   </sheetData>
@@ -8243,7 +8269,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11035,6 +11061,19 @@
       </c>
       <c r="C214" t="n">
         <v>53.33</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="8" t="n">
+        <v>45885</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>53.37</v>
       </c>
     </row>
   </sheetData>
@@ -11048,7 +11087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13840,6 +13879,19 @@
       </c>
       <c r="C214" t="n">
         <v>53.61</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="8" t="n">
+        <v>45885</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>53.65</v>
       </c>
     </row>
   </sheetData>
@@ -13853,7 +13905,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16645,6 +16697,19 @@
       </c>
       <c r="C214" t="n">
         <v>54.34</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="8" t="n">
+        <v>45885</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>54.38</v>
       </c>
     </row>
   </sheetData>
@@ -16658,7 +16723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19450,6 +19515,19 @@
       </c>
       <c r="C214" t="n">
         <v>54.02</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="8" t="n">
+        <v>45885</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>54.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-19 02:26:56
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-16</t>
+          <t>2025-08-19</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-16</t>
+          <t>2025-08-19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-16</t>
+          <t>2025-08-19</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-16</t>
+          <t>2025-08-19</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-16</t>
+          <t>2025-08-19</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-16</t>
+          <t>2025-08-19</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C215"/>
+  <dimension ref="A1:C216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5437,6 +5437,19 @@
         </is>
       </c>
       <c r="C215" t="n">
+        <v>52.11</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="8" t="n">
+        <v>45888</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
         <v>52.11</v>
       </c>
     </row>
@@ -5451,7 +5464,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C215"/>
+  <dimension ref="A1:C216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8255,6 +8268,19 @@
         </is>
       </c>
       <c r="C215" t="n">
+        <v>54.43</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="8" t="n">
+        <v>45888</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
         <v>54.43</v>
       </c>
     </row>
@@ -8269,7 +8295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C215"/>
+  <dimension ref="A1:C216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11073,6 +11099,19 @@
         </is>
       </c>
       <c r="C215" t="n">
+        <v>53.37</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="8" t="n">
+        <v>45888</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
         <v>53.37</v>
       </c>
     </row>
@@ -11087,7 +11126,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C215"/>
+  <dimension ref="A1:C216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13891,6 +13930,19 @@
         </is>
       </c>
       <c r="C215" t="n">
+        <v>53.65</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="8" t="n">
+        <v>45888</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
         <v>53.65</v>
       </c>
     </row>
@@ -13905,7 +13957,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C215"/>
+  <dimension ref="A1:C216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16709,6 +16761,19 @@
         </is>
       </c>
       <c r="C215" t="n">
+        <v>54.38</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="8" t="n">
+        <v>45888</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
         <v>54.38</v>
       </c>
     </row>
@@ -16723,7 +16788,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C215"/>
+  <dimension ref="A1:C216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19527,6 +19592,19 @@
         </is>
       </c>
       <c r="C215" t="n">
+        <v>54.06</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="8" t="n">
+        <v>45888</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
         <v>54.06</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-22 02:25:31
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-19</t>
+          <t>2025-08-22</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-19</t>
+          <t>2025-08-22</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-19</t>
+          <t>2025-08-22</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-19</t>
+          <t>2025-08-22</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-19</t>
+          <t>2025-08-22</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-19</t>
+          <t>2025-08-22</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C216"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5451,6 +5451,19 @@
       </c>
       <c r="C216" t="n">
         <v>52.11</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="8" t="n">
+        <v>45891</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>52.14</v>
       </c>
     </row>
   </sheetData>
@@ -5464,7 +5477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C216"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8282,6 +8295,19 @@
       </c>
       <c r="C216" t="n">
         <v>54.43</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="8" t="n">
+        <v>45891</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>54.48</v>
       </c>
     </row>
   </sheetData>
@@ -8295,7 +8321,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C216"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11113,6 +11139,19 @@
       </c>
       <c r="C216" t="n">
         <v>53.37</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="8" t="n">
+        <v>45891</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>53.42</v>
       </c>
     </row>
   </sheetData>
@@ -11126,7 +11165,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C216"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13944,6 +13983,19 @@
       </c>
       <c r="C216" t="n">
         <v>53.65</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="8" t="n">
+        <v>45891</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>53.69</v>
       </c>
     </row>
   </sheetData>
@@ -13957,7 +14009,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C216"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16775,6 +16827,19 @@
       </c>
       <c r="C216" t="n">
         <v>54.38</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="8" t="n">
+        <v>45891</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>54.43</v>
       </c>
     </row>
   </sheetData>
@@ -16788,7 +16853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C216"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19606,6 +19671,19 @@
       </c>
       <c r="C216" t="n">
         <v>54.06</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="8" t="n">
+        <v>45891</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>54.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-27 02:21:00
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-08-27</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-08-27</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-08-27</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-08-27</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-08-27</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-08-27</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C217"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5463,6 +5463,19 @@
         </is>
       </c>
       <c r="C217" t="n">
+        <v>52.14</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="8" t="n">
+        <v>45896</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
         <v>52.14</v>
       </c>
     </row>
@@ -5477,7 +5490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C217"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8307,6 +8320,19 @@
         </is>
       </c>
       <c r="C217" t="n">
+        <v>54.48</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="8" t="n">
+        <v>45896</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
         <v>54.48</v>
       </c>
     </row>
@@ -8321,7 +8347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C217"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11151,6 +11177,19 @@
         </is>
       </c>
       <c r="C217" t="n">
+        <v>53.42</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="8" t="n">
+        <v>45896</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
         <v>53.42</v>
       </c>
     </row>
@@ -11165,7 +11204,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C217"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13995,6 +14034,19 @@
         </is>
       </c>
       <c r="C217" t="n">
+        <v>53.69</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="8" t="n">
+        <v>45896</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
         <v>53.69</v>
       </c>
     </row>
@@ -14009,7 +14061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C217"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16839,6 +16891,19 @@
         </is>
       </c>
       <c r="C217" t="n">
+        <v>54.43</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="8" t="n">
+        <v>45896</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
         <v>54.43</v>
       </c>
     </row>
@@ -16853,7 +16918,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C217"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19683,6 +19748,19 @@
         </is>
       </c>
       <c r="C217" t="n">
+        <v>54.11</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="8" t="n">
+        <v>45896</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
         <v>54.11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-28 02:20:21
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-08-28</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-08-28</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-08-28</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-08-28</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-08-28</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-08-28</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5476,6 +5476,19 @@
         </is>
       </c>
       <c r="C218" t="n">
+        <v>52.14</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="8" t="n">
+        <v>45897</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
         <v>52.14</v>
       </c>
     </row>
@@ -5490,7 +5503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8333,6 +8346,19 @@
         </is>
       </c>
       <c r="C218" t="n">
+        <v>54.48</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="8" t="n">
+        <v>45897</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
         <v>54.48</v>
       </c>
     </row>
@@ -8347,7 +8373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11190,6 +11216,19 @@
         </is>
       </c>
       <c r="C218" t="n">
+        <v>53.42</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="8" t="n">
+        <v>45897</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
         <v>53.42</v>
       </c>
     </row>
@@ -11204,7 +11243,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14047,6 +14086,19 @@
         </is>
       </c>
       <c r="C218" t="n">
+        <v>53.69</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="8" t="n">
+        <v>45897</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
         <v>53.69</v>
       </c>
     </row>
@@ -14061,7 +14113,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16904,6 +16956,19 @@
         </is>
       </c>
       <c r="C218" t="n">
+        <v>54.43</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="8" t="n">
+        <v>45897</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
         <v>54.43</v>
       </c>
     </row>
@@ -16918,7 +16983,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19761,6 +19826,19 @@
         </is>
       </c>
       <c r="C218" t="n">
+        <v>54.11</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="8" t="n">
+        <v>45897</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
         <v>54.11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-08-29 02:20:49
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-08-29</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-08-29</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-08-29</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-08-29</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-08-29</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-08-29</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5490,6 +5490,19 @@
       </c>
       <c r="C219" t="n">
         <v>52.14</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="8" t="n">
+        <v>45898</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>52.17</v>
       </c>
     </row>
   </sheetData>
@@ -5503,7 +5516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8360,6 +8373,19 @@
       </c>
       <c r="C219" t="n">
         <v>54.48</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="8" t="n">
+        <v>45898</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>54.53</v>
       </c>
     </row>
   </sheetData>
@@ -8373,7 +8399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11230,6 +11256,19 @@
       </c>
       <c r="C219" t="n">
         <v>53.42</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="8" t="n">
+        <v>45898</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>53.45</v>
       </c>
     </row>
   </sheetData>
@@ -11243,7 +11282,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14100,6 +14139,19 @@
       </c>
       <c r="C219" t="n">
         <v>53.69</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="8" t="n">
+        <v>45898</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>53.74</v>
       </c>
     </row>
   </sheetData>
@@ -14113,7 +14165,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16970,6 +17022,19 @@
       </c>
       <c r="C219" t="n">
         <v>54.43</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="8" t="n">
+        <v>45898</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>54.48</v>
       </c>
     </row>
   </sheetData>
@@ -16983,7 +17048,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19840,6 +19905,19 @@
       </c>
       <c r="C219" t="n">
         <v>54.11</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="8" t="n">
+        <v>45898</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>54.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-02 02:22:59
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-02</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-02</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-02</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5503,6 +5503,19 @@
       </c>
       <c r="C220" t="n">
         <v>52.17</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="8" t="n">
+        <v>45902</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>52.18</v>
       </c>
     </row>
   </sheetData>
@@ -5516,7 +5529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8386,6 +8399,19 @@
       </c>
       <c r="C220" t="n">
         <v>54.53</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="8" t="n">
+        <v>45902</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>54.54</v>
       </c>
     </row>
   </sheetData>
@@ -8399,7 +8425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11269,6 +11295,19 @@
       </c>
       <c r="C220" t="n">
         <v>53.45</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="8" t="n">
+        <v>45902</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>53.46</v>
       </c>
     </row>
   </sheetData>
@@ -11282,7 +11321,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14152,6 +14191,19 @@
       </c>
       <c r="C220" t="n">
         <v>53.74</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="8" t="n">
+        <v>45902</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>53.75</v>
       </c>
     </row>
   </sheetData>
@@ -14165,7 +14217,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17035,6 +17087,19 @@
       </c>
       <c r="C220" t="n">
         <v>54.48</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="8" t="n">
+        <v>45902</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>54.49</v>
       </c>
     </row>
   </sheetData>
@@ -17048,7 +17113,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19918,6 +19983,19 @@
       </c>
       <c r="C220" t="n">
         <v>54.16</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="8" t="n">
+        <v>45902</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>54.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-03 02:13:38
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-09-03</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-09-03</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-09-03</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-09-03</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-09-03</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-09-03</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C221"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5516,6 +5516,19 @@
       </c>
       <c r="C221" t="n">
         <v>52.18</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="8" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>52.21</v>
       </c>
     </row>
   </sheetData>
@@ -5529,7 +5542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C221"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8412,6 +8425,19 @@
       </c>
       <c r="C221" t="n">
         <v>54.54</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="8" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>54.59</v>
       </c>
     </row>
   </sheetData>
@@ -8425,7 +8451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C221"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11308,6 +11334,19 @@
       </c>
       <c r="C221" t="n">
         <v>53.46</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="8" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>53.51</v>
       </c>
     </row>
   </sheetData>
@@ -11321,7 +11360,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C221"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14204,6 +14243,19 @@
       </c>
       <c r="C221" t="n">
         <v>53.75</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="8" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>53.8</v>
       </c>
     </row>
   </sheetData>
@@ -14217,7 +14269,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C221"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17100,6 +17152,19 @@
       </c>
       <c r="C221" t="n">
         <v>54.49</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="8" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>54.54</v>
       </c>
     </row>
   </sheetData>
@@ -17113,7 +17178,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C221"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19996,6 +20061,19 @@
       </c>
       <c r="C221" t="n">
         <v>54.17</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="8" t="n">
+        <v>45903</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>54.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-04 02:14:04
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5529,6 +5529,19 @@
       </c>
       <c r="C222" t="n">
         <v>52.21</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="8" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>54.26</v>
       </c>
     </row>
   </sheetData>
@@ -5542,7 +5555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8438,6 +8451,19 @@
       </c>
       <c r="C222" t="n">
         <v>54.59</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="8" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>56.64</v>
       </c>
     </row>
   </sheetData>
@@ -8451,7 +8477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11347,6 +11373,19 @@
       </c>
       <c r="C222" t="n">
         <v>53.51</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="8" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>55.56</v>
       </c>
     </row>
   </sheetData>
@@ -11360,7 +11399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14256,6 +14295,19 @@
       </c>
       <c r="C222" t="n">
         <v>53.8</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="8" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>55.85</v>
       </c>
     </row>
   </sheetData>
@@ -14269,7 +14321,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17165,6 +17217,19 @@
       </c>
       <c r="C222" t="n">
         <v>54.54</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="8" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>56.59</v>
       </c>
     </row>
   </sheetData>
@@ -17178,7 +17243,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C222"/>
+  <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20074,6 +20139,19 @@
       </c>
       <c r="C222" t="n">
         <v>54.22</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="8" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>56.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-06 02:13:21
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>2025-09-06</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>2025-09-06</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>2025-09-06</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>2025-09-06</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>2025-09-06</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>2025-09-06</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5542,6 +5542,19 @@
       </c>
       <c r="C223" t="n">
         <v>54.26</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="8" t="n">
+        <v>45906</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>54.31</v>
       </c>
     </row>
   </sheetData>
@@ -5555,7 +5568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8464,6 +8477,19 @@
       </c>
       <c r="C223" t="n">
         <v>56.64</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="8" t="n">
+        <v>45906</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>56.71</v>
       </c>
     </row>
   </sheetData>
@@ -8477,7 +8503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11386,6 +11412,19 @@
       </c>
       <c r="C223" t="n">
         <v>55.56</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="8" t="n">
+        <v>45906</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>55.63</v>
       </c>
     </row>
   </sheetData>
@@ -11399,7 +11438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14308,6 +14347,19 @@
       </c>
       <c r="C223" t="n">
         <v>55.85</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="8" t="n">
+        <v>45906</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>55.92</v>
       </c>
     </row>
   </sheetData>
@@ -14321,7 +14373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17230,6 +17282,19 @@
       </c>
       <c r="C223" t="n">
         <v>56.59</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="8" t="n">
+        <v>45906</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>56.66</v>
       </c>
     </row>
   </sheetData>
@@ -17243,7 +17308,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20152,6 +20217,19 @@
       </c>
       <c r="C223" t="n">
         <v>56.27</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="8" t="n">
+        <v>45906</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>56.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-09 02:19:27
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-06</t>
+          <t>2025-09-09</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-06</t>
+          <t>2025-09-09</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-06</t>
+          <t>2025-09-09</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-06</t>
+          <t>2025-09-09</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-06</t>
+          <t>2025-09-09</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-06</t>
+          <t>2025-09-09</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5554,6 +5554,19 @@
         </is>
       </c>
       <c r="C224" t="n">
+        <v>54.31</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="8" t="n">
+        <v>45909</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
         <v>54.31</v>
       </c>
     </row>
@@ -5568,7 +5581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8489,6 +8502,19 @@
         </is>
       </c>
       <c r="C224" t="n">
+        <v>56.71</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="8" t="n">
+        <v>45909</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
         <v>56.71</v>
       </c>
     </row>
@@ -8503,7 +8529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11424,6 +11450,19 @@
         </is>
       </c>
       <c r="C224" t="n">
+        <v>55.63</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="8" t="n">
+        <v>45909</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
         <v>55.63</v>
       </c>
     </row>
@@ -11438,7 +11477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14359,6 +14398,19 @@
         </is>
       </c>
       <c r="C224" t="n">
+        <v>55.92</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="8" t="n">
+        <v>45909</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
         <v>55.92</v>
       </c>
     </row>
@@ -14373,7 +14425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17294,6 +17346,19 @@
         </is>
       </c>
       <c r="C224" t="n">
+        <v>56.66</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="8" t="n">
+        <v>45909</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
         <v>56.66</v>
       </c>
     </row>
@@ -17308,7 +17373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C224"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20229,6 +20294,19 @@
         </is>
       </c>
       <c r="C224" t="n">
+        <v>56.36</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="8" t="n">
+        <v>45909</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
         <v>56.36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-11 02:18:13
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-11</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C225"/>
+  <dimension ref="A1:C226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5568,6 +5568,19 @@
       </c>
       <c r="C225" t="n">
         <v>54.31</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="8" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>54.36</v>
       </c>
     </row>
   </sheetData>
@@ -5581,7 +5594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C225"/>
+  <dimension ref="A1:C226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8516,6 +8529,19 @@
       </c>
       <c r="C225" t="n">
         <v>56.71</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="8" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>56.76</v>
       </c>
     </row>
   </sheetData>
@@ -8529,7 +8555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C225"/>
+  <dimension ref="A1:C226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11464,6 +11490,19 @@
       </c>
       <c r="C225" t="n">
         <v>55.63</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="8" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>55.68</v>
       </c>
     </row>
   </sheetData>
@@ -11477,7 +11516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C225"/>
+  <dimension ref="A1:C226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14412,6 +14451,19 @@
       </c>
       <c r="C225" t="n">
         <v>55.92</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="8" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>55.97</v>
       </c>
     </row>
   </sheetData>
@@ -14425,7 +14477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C225"/>
+  <dimension ref="A1:C226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17360,6 +17412,19 @@
       </c>
       <c r="C225" t="n">
         <v>56.66</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="8" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>56.71</v>
       </c>
     </row>
   </sheetData>
@@ -17373,7 +17438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C225"/>
+  <dimension ref="A1:C226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20308,6 +20373,19 @@
       </c>
       <c r="C225" t="n">
         <v>56.36</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="8" t="n">
+        <v>45911</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>56.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-16 02:14:42
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5581,6 +5581,19 @@
       </c>
       <c r="C226" t="n">
         <v>54.36</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="8" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>54.4</v>
       </c>
     </row>
   </sheetData>
@@ -5594,7 +5607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8542,6 +8555,19 @@
       </c>
       <c r="C226" t="n">
         <v>56.76</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="8" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>56.81</v>
       </c>
     </row>
   </sheetData>
@@ -8555,7 +8581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11503,6 +11529,19 @@
       </c>
       <c r="C226" t="n">
         <v>55.68</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="8" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>55.73</v>
       </c>
     </row>
   </sheetData>
@@ -11516,7 +11555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14464,6 +14503,19 @@
       </c>
       <c r="C226" t="n">
         <v>55.97</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="8" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>56.02</v>
       </c>
     </row>
   </sheetData>
@@ -14477,7 +14529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17425,6 +17477,19 @@
       </c>
       <c r="C226" t="n">
         <v>56.71</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="8" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>56.76</v>
       </c>
     </row>
   </sheetData>
@@ -17438,7 +17503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C226"/>
+  <dimension ref="A1:C227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20386,6 +20451,19 @@
       </c>
       <c r="C226" t="n">
         <v>56.41</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="8" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>56.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-23 02:15:13
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C227"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5594,6 +5594,19 @@
       </c>
       <c r="C227" t="n">
         <v>54.4</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="8" t="n">
+        <v>45923</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>54.43</v>
       </c>
     </row>
   </sheetData>
@@ -5607,7 +5620,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C227"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8568,6 +8581,19 @@
       </c>
       <c r="C227" t="n">
         <v>56.81</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="8" t="n">
+        <v>45923</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>56.84</v>
       </c>
     </row>
   </sheetData>
@@ -8581,7 +8607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C227"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11542,6 +11568,19 @@
       </c>
       <c r="C227" t="n">
         <v>55.73</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="8" t="n">
+        <v>45923</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>55.76</v>
       </c>
     </row>
   </sheetData>
@@ -11555,7 +11594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C227"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14516,6 +14555,19 @@
       </c>
       <c r="C227" t="n">
         <v>56.02</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="8" t="n">
+        <v>45923</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>56.05</v>
       </c>
     </row>
   </sheetData>
@@ -14529,7 +14581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C227"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17490,6 +17542,19 @@
       </c>
       <c r="C227" t="n">
         <v>56.76</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="8" t="n">
+        <v>45923</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>56.79</v>
       </c>
     </row>
   </sheetData>
@@ -17503,7 +17568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C227"/>
+  <dimension ref="A1:C228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20464,6 +20529,19 @@
       </c>
       <c r="C227" t="n">
         <v>56.46</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="8" t="n">
+        <v>45923</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>56.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-26 02:17:40
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C228"/>
+  <dimension ref="A1:C229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5606,6 +5606,19 @@
         </is>
       </c>
       <c r="C228" t="n">
+        <v>54.43</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="8" t="n">
+        <v>45926</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
         <v>54.43</v>
       </c>
     </row>
@@ -5620,7 +5633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C228"/>
+  <dimension ref="A1:C229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8593,6 +8606,19 @@
         </is>
       </c>
       <c r="C228" t="n">
+        <v>56.84</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="8" t="n">
+        <v>45926</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
         <v>56.84</v>
       </c>
     </row>
@@ -8607,7 +8633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C228"/>
+  <dimension ref="A1:C229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11580,6 +11606,19 @@
         </is>
       </c>
       <c r="C228" t="n">
+        <v>55.76</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="8" t="n">
+        <v>45926</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
         <v>55.76</v>
       </c>
     </row>
@@ -11594,7 +11633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C228"/>
+  <dimension ref="A1:C229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14567,6 +14606,19 @@
         </is>
       </c>
       <c r="C228" t="n">
+        <v>56.05</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="8" t="n">
+        <v>45926</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
         <v>56.05</v>
       </c>
     </row>
@@ -14581,7 +14633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C228"/>
+  <dimension ref="A1:C229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17554,6 +17606,19 @@
         </is>
       </c>
       <c r="C228" t="n">
+        <v>56.79</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="8" t="n">
+        <v>45926</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
         <v>56.79</v>
       </c>
     </row>
@@ -17568,7 +17633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C228"/>
+  <dimension ref="A1:C229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20541,6 +20606,19 @@
         </is>
       </c>
       <c r="C228" t="n">
+        <v>56.49</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="8" t="n">
+        <v>45926</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
         <v>56.49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-27 02:12:09
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5620,6 +5620,19 @@
       </c>
       <c r="C229" t="n">
         <v>54.43</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="8" t="n">
+        <v>45927</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>54.45</v>
       </c>
     </row>
   </sheetData>
@@ -5633,7 +5646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8620,6 +8633,19 @@
       </c>
       <c r="C229" t="n">
         <v>56.84</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="8" t="n">
+        <v>45927</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>56.87</v>
       </c>
     </row>
   </sheetData>
@@ -8633,7 +8659,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11620,6 +11646,19 @@
       </c>
       <c r="C229" t="n">
         <v>55.76</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="8" t="n">
+        <v>45927</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>55.79</v>
       </c>
     </row>
   </sheetData>
@@ -11633,7 +11672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14620,6 +14659,19 @@
       </c>
       <c r="C229" t="n">
         <v>56.05</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="8" t="n">
+        <v>45927</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>56.08</v>
       </c>
     </row>
   </sheetData>
@@ -14633,7 +14685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17620,6 +17672,19 @@
       </c>
       <c r="C229" t="n">
         <v>56.79</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="8" t="n">
+        <v>45927</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>56.82</v>
       </c>
     </row>
   </sheetData>
@@ -17633,7 +17698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20620,6 +20685,19 @@
       </c>
       <c r="C229" t="n">
         <v>56.49</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="8" t="n">
+        <v>45927</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>56.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-09-30 02:15:27
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C230"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5632,6 +5632,19 @@
         </is>
       </c>
       <c r="C230" t="n">
+        <v>54.45</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="8" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
         <v>54.45</v>
       </c>
     </row>
@@ -5646,7 +5659,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C230"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8645,6 +8658,19 @@
         </is>
       </c>
       <c r="C230" t="n">
+        <v>56.87</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="8" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
         <v>56.87</v>
       </c>
     </row>
@@ -8659,7 +8685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C230"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11658,6 +11684,19 @@
         </is>
       </c>
       <c r="C230" t="n">
+        <v>55.79</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="8" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
         <v>55.79</v>
       </c>
     </row>
@@ -11672,7 +11711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C230"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14671,6 +14710,19 @@
         </is>
       </c>
       <c r="C230" t="n">
+        <v>56.08</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="8" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
         <v>56.08</v>
       </c>
     </row>
@@ -14685,7 +14737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C230"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17684,6 +17736,19 @@
         </is>
       </c>
       <c r="C230" t="n">
+        <v>56.82</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="8" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
         <v>56.82</v>
       </c>
     </row>
@@ -17698,7 +17763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C230"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20697,6 +20762,19 @@
         </is>
       </c>
       <c r="C230" t="n">
+        <v>56.52</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="8" t="n">
+        <v>45930</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
         <v>56.52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-10-01 02:27:30
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C231"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5645,6 +5645,19 @@
         </is>
       </c>
       <c r="C231" t="n">
+        <v>54.45</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="8" t="n">
+        <v>45931</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
         <v>54.45</v>
       </c>
     </row>
@@ -5659,7 +5672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C231"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8671,6 +8684,19 @@
         </is>
       </c>
       <c r="C231" t="n">
+        <v>56.87</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="8" t="n">
+        <v>45931</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
         <v>56.87</v>
       </c>
     </row>
@@ -8685,7 +8711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C231"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11697,6 +11723,19 @@
         </is>
       </c>
       <c r="C231" t="n">
+        <v>55.79</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="8" t="n">
+        <v>45931</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
         <v>55.79</v>
       </c>
     </row>
@@ -11711,7 +11750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C231"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14723,6 +14762,19 @@
         </is>
       </c>
       <c r="C231" t="n">
+        <v>56.08</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="8" t="n">
+        <v>45931</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
         <v>56.08</v>
       </c>
     </row>
@@ -14737,7 +14789,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C231"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17749,6 +17801,19 @@
         </is>
       </c>
       <c r="C231" t="n">
+        <v>56.82</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="8" t="n">
+        <v>45931</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
         <v>56.82</v>
       </c>
     </row>
@@ -17763,7 +17828,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C231"/>
+  <dimension ref="A1:C232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20775,6 +20840,19 @@
         </is>
       </c>
       <c r="C231" t="n">
+        <v>56.52</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="8" t="n">
+        <v>45931</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
         <v>56.52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-10-02 02:15:01
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5659,6 +5659,19 @@
       </c>
       <c r="C232" t="n">
         <v>54.45</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="8" t="n">
+        <v>45932</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>54.46</v>
       </c>
     </row>
   </sheetData>
@@ -5672,7 +5685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8698,6 +8711,19 @@
       </c>
       <c r="C232" t="n">
         <v>56.87</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="8" t="n">
+        <v>45932</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>56.88</v>
       </c>
     </row>
   </sheetData>
@@ -8711,7 +8737,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11737,6 +11763,19 @@
       </c>
       <c r="C232" t="n">
         <v>55.79</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="8" t="n">
+        <v>45932</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>55.8</v>
       </c>
     </row>
   </sheetData>
@@ -11750,7 +11789,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14776,6 +14815,19 @@
       </c>
       <c r="C232" t="n">
         <v>56.08</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="8" t="n">
+        <v>45932</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>56.09</v>
       </c>
     </row>
   </sheetData>
@@ -14789,7 +14841,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17815,6 +17867,19 @@
       </c>
       <c r="C232" t="n">
         <v>56.82</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="8" t="n">
+        <v>45932</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>56.83</v>
       </c>
     </row>
   </sheetData>
@@ -17828,7 +17893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C232"/>
+  <dimension ref="A1:C233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20854,6 +20919,19 @@
       </c>
       <c r="C232" t="n">
         <v>56.52</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="8" t="n">
+        <v>45932</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>56.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-10-03 02:14:39
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C233"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5672,6 +5672,19 @@
       </c>
       <c r="C233" t="n">
         <v>54.46</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="8" t="n">
+        <v>45933</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>54.5</v>
       </c>
     </row>
   </sheetData>
@@ -5685,7 +5698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C233"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8724,6 +8737,19 @@
       </c>
       <c r="C233" t="n">
         <v>56.88</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="8" t="n">
+        <v>45933</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>56.93</v>
       </c>
     </row>
   </sheetData>
@@ -8737,7 +8763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C233"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11776,6 +11802,19 @@
       </c>
       <c r="C233" t="n">
         <v>55.8</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="8" t="n">
+        <v>45933</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>55.85</v>
       </c>
     </row>
   </sheetData>
@@ -11789,7 +11828,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C233"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14828,6 +14867,19 @@
       </c>
       <c r="C233" t="n">
         <v>56.09</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="8" t="n">
+        <v>45933</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>56.14</v>
       </c>
     </row>
   </sheetData>
@@ -14841,7 +14893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C233"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17880,6 +17932,19 @@
       </c>
       <c r="C233" t="n">
         <v>56.83</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="8" t="n">
+        <v>45933</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>56.88</v>
       </c>
     </row>
   </sheetData>
@@ -17893,7 +17958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C233"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20932,6 +20997,19 @@
       </c>
       <c r="C233" t="n">
         <v>56.53</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="8" t="n">
+        <v>45933</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>56.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Otomatik güncelleme: 2025-10-04 02:10:05
</commit_message>
<xml_diff>
--- a/Veri1.xlsx
+++ b/Veri1.xlsx
@@ -2528,7 +2528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C234"/>
+  <dimension ref="A1:C235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5684,6 +5684,19 @@
         </is>
       </c>
       <c r="C234" t="n">
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="8" t="n">
+        <v>45934</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
         <v>54.5</v>
       </c>
     </row>
@@ -5698,7 +5711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C234"/>
+  <dimension ref="A1:C235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8749,6 +8762,19 @@
         </is>
       </c>
       <c r="C234" t="n">
+        <v>56.93</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="8" t="n">
+        <v>45934</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
         <v>56.93</v>
       </c>
     </row>
@@ -8763,7 +8789,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C234"/>
+  <dimension ref="A1:C235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11814,6 +11840,19 @@
         </is>
       </c>
       <c r="C234" t="n">
+        <v>55.85</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="8" t="n">
+        <v>45934</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
         <v>55.85</v>
       </c>
     </row>
@@ -11828,7 +11867,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C234"/>
+  <dimension ref="A1:C235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14879,6 +14918,19 @@
         </is>
       </c>
       <c r="C234" t="n">
+        <v>56.14</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="8" t="n">
+        <v>45934</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
         <v>56.14</v>
       </c>
     </row>
@@ -14893,7 +14945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C234"/>
+  <dimension ref="A1:C235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17944,6 +17996,19 @@
         </is>
       </c>
       <c r="C234" t="n">
+        <v>56.88</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="8" t="n">
+        <v>45934</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
         <v>56.88</v>
       </c>
     </row>
@@ -17958,7 +18023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C234"/>
+  <dimension ref="A1:C235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21009,6 +21074,19 @@
         </is>
       </c>
       <c r="C234" t="n">
+        <v>56.58</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="8" t="n">
+        <v>45934</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
         <v>56.58</v>
       </c>
     </row>

</xml_diff>